<commit_message>
Release of 0.1.5 BETA.
</commit_message>
<xml_diff>
--- a/SUEWSPrepare/Input/SUEWS_SiteSelect.xlsx
+++ b/SUEWSPrepare/Input/SUEWS_SiteSelect.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="232">
   <si>
     <t>Grid</t>
   </si>
@@ -663,13 +663,64 @@
   </si>
   <si>
     <t>ID attribute</t>
+  </si>
+  <si>
+    <t>wallarea</t>
+  </si>
+  <si>
+    <t>fLUb1</t>
+  </si>
+  <si>
+    <t>Code_LUbuilding1</t>
+  </si>
+  <si>
+    <t>fLUb2</t>
+  </si>
+  <si>
+    <t>Code_LUbuilding2</t>
+  </si>
+  <si>
+    <t>fLUb3</t>
+  </si>
+  <si>
+    <t>Code_LUbuilding3</t>
+  </si>
+  <si>
+    <t>fLUb4</t>
+  </si>
+  <si>
+    <t>Code_LUbuilding4</t>
+  </si>
+  <si>
+    <t>fLUb5</t>
+  </si>
+  <si>
+    <t>Code_LUbuilding5</t>
+  </si>
+  <si>
+    <t>fLUp1</t>
+  </si>
+  <si>
+    <t>Code_LUpaved1</t>
+  </si>
+  <si>
+    <t>fLUp2</t>
+  </si>
+  <si>
+    <t>Code_LUpaved2</t>
+  </si>
+  <si>
+    <t>fLUp3</t>
+  </si>
+  <si>
+    <t>Code_LUpaved3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -801,6 +852,19 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1159,12 +1223,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1507,10 +1573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CE88"/>
+  <dimension ref="A1:CV88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" topLeftCell="CB1" workbookViewId="0">
+      <selection activeCell="CM31" sqref="CM31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1520,7 +1586,7 @@
     <col min="41" max="41" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -1761,8 +1827,59 @@
       <c r="CB1">
         <v>80</v>
       </c>
-    </row>
-    <row r="2" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CC1">
+        <v>81</v>
+      </c>
+      <c r="CD1">
+        <v>82</v>
+      </c>
+      <c r="CE1">
+        <v>83</v>
+      </c>
+      <c r="CF1">
+        <v>84</v>
+      </c>
+      <c r="CG1">
+        <v>85</v>
+      </c>
+      <c r="CH1">
+        <v>86</v>
+      </c>
+      <c r="CI1">
+        <v>87</v>
+      </c>
+      <c r="CJ1">
+        <v>88</v>
+      </c>
+      <c r="CK1">
+        <v>89</v>
+      </c>
+      <c r="CL1">
+        <v>90</v>
+      </c>
+      <c r="CM1">
+        <v>91</v>
+      </c>
+      <c r="CN1">
+        <v>92</v>
+      </c>
+      <c r="CO1">
+        <v>93</v>
+      </c>
+      <c r="CP1">
+        <v>94</v>
+      </c>
+      <c r="CQ1">
+        <v>95</v>
+      </c>
+      <c r="CR1">
+        <v>96</v>
+      </c>
+      <c r="CS1">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2003,8 +2120,59 @@
       <c r="CB2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="3" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CC2" t="s">
+        <v>215</v>
+      </c>
+      <c r="CD2" t="s">
+        <v>216</v>
+      </c>
+      <c r="CE2" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="CF2" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="CG2" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="CH2" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="CI2" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="CJ2" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="CK2" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="CL2" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="CM2" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="CN2" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="CO2" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="CP2" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="CQ2" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="CR2" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="CS2" s="5" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="3" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2245,62 +2413,113 @@
       <c r="CB3">
         <v>667</v>
       </c>
-      <c r="CC3" t="s">
-        <v>80</v>
-      </c>
-      <c r="CD3" t="s">
+      <c r="CC3" s="5">
+        <v>1.27</v>
+      </c>
+      <c r="CD3" s="6">
+        <v>0.15</v>
+      </c>
+      <c r="CE3" s="5">
+        <v>801</v>
+      </c>
+      <c r="CF3" s="5">
+        <v>0.45</v>
+      </c>
+      <c r="CG3" s="5">
+        <v>802</v>
+      </c>
+      <c r="CH3" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="CI3" s="5">
+        <v>803</v>
+      </c>
+      <c r="CJ3" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="CK3" s="5">
+        <v>804</v>
+      </c>
+      <c r="CL3" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="CM3" s="5">
+        <v>805</v>
+      </c>
+      <c r="CN3" s="5">
+        <v>0.15</v>
+      </c>
+      <c r="CO3" s="5">
+        <v>806</v>
+      </c>
+      <c r="CP3" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="CQ3" s="5">
+        <v>807</v>
+      </c>
+      <c r="CR3" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="CS3" s="5">
+        <v>808</v>
+      </c>
+      <c r="CT3" t="s">
+        <v>80</v>
+      </c>
+      <c r="CU3" t="s">
         <v>81</v>
       </c>
-      <c r="CE3" t="s">
+      <c r="CV3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>-9</v>
       </c>
     </row>
-    <row r="5" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>-9</v>
       </c>
     </row>
-    <row r="9" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>80</v>
       </c>

</xml_diff>

<commit_message>
Bug fixes for SUEWSPrepare and SUEWSSimple
</commit_message>
<xml_diff>
--- a/SUEWSPrepare/Input/SUEWS_SiteSelect.xlsx
+++ b/SUEWSPrepare/Input/SUEWS_SiteSelect.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="234">
   <si>
     <t>Grid</t>
   </si>
@@ -266,9 +266,6 @@
     <t>London</t>
   </si>
   <si>
-    <t>Kotthaus &amp; Grimmond (2012)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Grid </t>
   </si>
   <si>
@@ -665,62 +662,71 @@
     <t>ID attribute</t>
   </si>
   <si>
-    <t>wallarea</t>
-  </si>
-  <si>
-    <t>fLUb1</t>
-  </si>
-  <si>
-    <t>Code_LUbuilding1</t>
-  </si>
-  <si>
-    <t>fLUb2</t>
-  </si>
-  <si>
-    <t>Code_LUbuilding2</t>
-  </si>
-  <si>
-    <t>fLUb3</t>
-  </si>
-  <si>
-    <t>Code_LUbuilding3</t>
-  </si>
-  <si>
-    <t>fLUb4</t>
-  </si>
-  <si>
-    <t>Code_LUbuilding4</t>
-  </si>
-  <si>
-    <t>fLUb5</t>
-  </si>
-  <si>
-    <t>Code_LUbuilding5</t>
-  </si>
-  <si>
-    <t>fLUp1</t>
-  </si>
-  <si>
-    <t>Code_LUpaved1</t>
-  </si>
-  <si>
-    <t>fLUp2</t>
-  </si>
-  <si>
-    <t>Code_LUpaved2</t>
-  </si>
-  <si>
-    <t>fLUp3</t>
-  </si>
-  <si>
-    <t>Code_LUpaved3</t>
+    <t>AreaWall</t>
+  </si>
+  <si>
+    <t>Fr_ESTMClass_Paved1</t>
+  </si>
+  <si>
+    <t>Fr_ESTMClass_Paved2</t>
+  </si>
+  <si>
+    <t>Fr_ESTMClass_Paved3</t>
+  </si>
+  <si>
+    <t>Code_ESTMClass_Paved1</t>
+  </si>
+  <si>
+    <t>Code_ESTMClass_Paved2</t>
+  </si>
+  <si>
+    <t>Code_ESTMClass_Paved3</t>
+  </si>
+  <si>
+    <t>Fr_ESTMClass_Bldgs1</t>
+  </si>
+  <si>
+    <t>Fr_ESTMClass_Bldgs2</t>
+  </si>
+  <si>
+    <t>Fr_ESTMClass_Bldgs3</t>
+  </si>
+  <si>
+    <t>Fr_ESTMClass_Bldgs4</t>
+  </si>
+  <si>
+    <t>Fr_ESTMClass_Bldgs5</t>
+  </si>
+  <si>
+    <t>Code_ESTMClass_Bldgs1</t>
+  </si>
+  <si>
+    <t>Code_ESTMClass_Bldgs2</t>
+  </si>
+  <si>
+    <t>Code_ESTMClass_Bldgs3</t>
+  </si>
+  <si>
+    <t>Code_ESTMClass_Bldgs4</t>
+  </si>
+  <si>
+    <t>Code_ESTMClass_Bldgs5</t>
+  </si>
+  <si>
+    <t>Site</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>Kotthaus and Grimmond (2013, 2014a, 2014b)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -852,19 +858,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1223,14 +1216,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1573,10 +1564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CV88"/>
+  <dimension ref="A1:CV83"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="CB1" workbookViewId="0">
-      <selection activeCell="CM31" sqref="CM31"/>
+      <selection activeCell="CC7" sqref="CC7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2121,55 +2112,64 @@
         <v>79</v>
       </c>
       <c r="CC2" t="s">
+        <v>214</v>
+      </c>
+      <c r="CD2" t="s">
         <v>215</v>
       </c>
-      <c r="CD2" t="s">
+      <c r="CE2" t="s">
         <v>216</v>
       </c>
-      <c r="CE2" s="5" t="s">
+      <c r="CF2" t="s">
         <v>217</v>
       </c>
-      <c r="CF2" s="5" t="s">
+      <c r="CG2" t="s">
         <v>218</v>
       </c>
-      <c r="CG2" s="5" t="s">
+      <c r="CH2" t="s">
         <v>219</v>
       </c>
-      <c r="CH2" s="5" t="s">
+      <c r="CI2" t="s">
         <v>220</v>
       </c>
-      <c r="CI2" s="5" t="s">
+      <c r="CJ2" t="s">
         <v>221</v>
       </c>
-      <c r="CJ2" s="5" t="s">
+      <c r="CK2" t="s">
         <v>222</v>
       </c>
-      <c r="CK2" s="5" t="s">
+      <c r="CL2" t="s">
         <v>223</v>
       </c>
-      <c r="CL2" s="5" t="s">
+      <c r="CM2" t="s">
         <v>224</v>
       </c>
-      <c r="CM2" s="5" t="s">
+      <c r="CN2" t="s">
         <v>225</v>
       </c>
-      <c r="CN2" s="5" t="s">
+      <c r="CO2" t="s">
         <v>226</v>
       </c>
-      <c r="CO2" s="5" t="s">
+      <c r="CP2" t="s">
         <v>227</v>
       </c>
-      <c r="CP2" s="5" t="s">
+      <c r="CQ2" t="s">
         <v>228</v>
       </c>
-      <c r="CQ2" s="5" t="s">
+      <c r="CR2" t="s">
         <v>229</v>
       </c>
-      <c r="CR2" s="5" t="s">
+      <c r="CS2" t="s">
         <v>230</v>
       </c>
-      <c r="CS2" s="5" t="s">
+      <c r="CT2" t="s">
+        <v>80</v>
+      </c>
+      <c r="CU2" t="s">
         <v>231</v>
+      </c>
+      <c r="CV2" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="3" spans="1:100" x14ac:dyDescent="0.25">
@@ -2264,28 +2264,28 @@
         <v>310.39999999999998</v>
       </c>
       <c r="AE3">
-        <v>98.76</v>
+        <v>204.6</v>
       </c>
       <c r="AF3">
-        <v>661</v>
+        <v>551</v>
       </c>
       <c r="AG3">
-        <v>662</v>
+        <v>552</v>
       </c>
       <c r="AH3">
-        <v>661</v>
+        <v>551</v>
       </c>
       <c r="AI3">
-        <v>662</v>
+        <v>552</v>
       </c>
       <c r="AJ3">
-        <v>663</v>
+        <v>553</v>
       </c>
       <c r="AK3">
-        <v>663</v>
+        <v>553</v>
       </c>
       <c r="AL3">
-        <v>661</v>
+        <v>551</v>
       </c>
       <c r="AM3">
         <v>0.25</v>
@@ -2312,13 +2312,13 @@
         <v>660</v>
       </c>
       <c r="AU3">
-        <v>661</v>
+        <v>551</v>
       </c>
       <c r="AV3">
-        <v>661</v>
+        <v>551</v>
       </c>
       <c r="AW3">
-        <v>662</v>
+        <v>552</v>
       </c>
       <c r="AX3">
         <v>660</v>
@@ -2393,76 +2393,76 @@
         <v>0</v>
       </c>
       <c r="BV3">
-        <v>661</v>
+        <v>551</v>
       </c>
       <c r="BW3">
-        <v>662</v>
+        <v>552</v>
       </c>
       <c r="BX3">
-        <v>663</v>
+        <v>553</v>
       </c>
       <c r="BY3">
-        <v>664</v>
+        <v>554</v>
       </c>
       <c r="BZ3">
-        <v>665</v>
+        <v>555</v>
       </c>
       <c r="CA3">
-        <v>666</v>
+        <v>556</v>
       </c>
       <c r="CB3">
-        <v>667</v>
-      </c>
-      <c r="CC3" s="5">
-        <v>1.27</v>
-      </c>
-      <c r="CD3" s="6">
+        <v>557</v>
+      </c>
+      <c r="CC3">
+        <v>950000</v>
+      </c>
+      <c r="CD3">
         <v>0.15</v>
       </c>
-      <c r="CE3" s="5">
+      <c r="CE3">
+        <v>0.05</v>
+      </c>
+      <c r="CF3">
+        <v>0.8</v>
+      </c>
+      <c r="CG3">
+        <v>806</v>
+      </c>
+      <c r="CH3">
+        <v>807</v>
+      </c>
+      <c r="CI3">
+        <v>808</v>
+      </c>
+      <c r="CJ3">
+        <v>0.15</v>
+      </c>
+      <c r="CK3">
+        <v>0.45</v>
+      </c>
+      <c r="CL3">
+        <v>0.05</v>
+      </c>
+      <c r="CM3">
+        <v>0.1</v>
+      </c>
+      <c r="CN3">
+        <v>0.25</v>
+      </c>
+      <c r="CO3">
         <v>801</v>
       </c>
-      <c r="CF3" s="5">
-        <v>0.45</v>
-      </c>
-      <c r="CG3" s="5">
+      <c r="CP3">
         <v>802</v>
       </c>
-      <c r="CH3" s="5">
-        <v>0.05</v>
-      </c>
-      <c r="CI3" s="5">
+      <c r="CQ3">
         <v>803</v>
       </c>
-      <c r="CJ3" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="CK3" s="5">
+      <c r="CR3">
         <v>804</v>
       </c>
-      <c r="CL3" s="5">
-        <v>0.25</v>
-      </c>
-      <c r="CM3" s="5">
+      <c r="CS3">
         <v>805</v>
-      </c>
-      <c r="CN3" s="5">
-        <v>0.15</v>
-      </c>
-      <c r="CO3" s="5">
-        <v>806</v>
-      </c>
-      <c r="CP3" s="5">
-        <v>0.05</v>
-      </c>
-      <c r="CQ3" s="5">
-        <v>807</v>
-      </c>
-      <c r="CR3" s="5">
-        <v>0.8</v>
-      </c>
-      <c r="CS3" s="5">
-        <v>808</v>
       </c>
       <c r="CT3" t="s">
         <v>80</v>
@@ -2471,7 +2471,7 @@
         <v>81</v>
       </c>
       <c r="CV3" t="s">
-        <v>82</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4" spans="1:100" x14ac:dyDescent="0.25">
@@ -2484,6 +2484,16 @@
         <v>-9</v>
       </c>
     </row>
+    <row r="7" spans="1:100" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:100" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>80</v>
+      </c>
+    </row>
     <row r="9" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>80</v>
@@ -2856,31 +2866,6 @@
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2913,28 +2898,28 @@
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>206</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2942,25 +2927,25 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2974,16 +2959,16 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -2994,19 +2979,19 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" t="s">
         <v>86</v>
       </c>
-      <c r="D4" t="s">
-        <v>87</v>
-      </c>
       <c r="E4" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="G4" t="s">
+        <v>185</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>182</v>
-      </c>
-      <c r="G4" t="s">
-        <v>186</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
@@ -3017,19 +3002,19 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E5" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="G5" t="s">
+        <v>185</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>182</v>
-      </c>
-      <c r="G5" t="s">
-        <v>186</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
@@ -3040,22 +3025,22 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" t="s">
         <v>89</v>
       </c>
-      <c r="D6" t="s">
-        <v>90</v>
-      </c>
       <c r="E6" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
@@ -3066,22 +3051,22 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -3095,19 +3080,19 @@
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -3118,22 +3103,22 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D9" t="s">
         <v>93</v>
       </c>
-      <c r="D9" t="s">
-        <v>94</v>
-      </c>
       <c r="E9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -3144,19 +3129,19 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H10" s="3"/>
     </row>
@@ -3168,16 +3153,16 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H11" s="3"/>
     </row>
@@ -3189,16 +3174,16 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F12" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H12" s="3"/>
     </row>
@@ -3210,16 +3195,16 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G13" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -3230,16 +3215,16 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -3250,16 +3235,16 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G15" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -3270,16 +3255,16 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G16" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -3290,16 +3275,16 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G17" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -3310,16 +3295,16 @@
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G18" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -3330,16 +3315,16 @@
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G19" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -3350,13 +3335,13 @@
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G20" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H20" s="3"/>
     </row>
@@ -3368,13 +3353,13 @@
         <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E21" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G21" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H21" s="3"/>
     </row>
@@ -3386,13 +3371,13 @@
         <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E22" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G22" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H22" s="3"/>
     </row>
@@ -3404,19 +3389,19 @@
         <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -3427,19 +3412,19 @@
         <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G24" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -3450,19 +3435,19 @@
         <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G25" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -3473,19 +3458,19 @@
         <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F26" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G26" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H26" s="3"/>
     </row>
@@ -3497,19 +3482,19 @@
         <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F27" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G27" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H27" s="3"/>
     </row>
@@ -3521,16 +3506,16 @@
         <v>26</v>
       </c>
       <c r="C28" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G28" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -3541,16 +3526,16 @@
         <v>27</v>
       </c>
       <c r="C29" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G29" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -3561,16 +3546,16 @@
         <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G30" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -3581,19 +3566,19 @@
         <v>29</v>
       </c>
       <c r="C31" t="s">
+        <v>109</v>
+      </c>
+      <c r="D31" t="s">
         <v>110</v>
       </c>
-      <c r="D31" t="s">
-        <v>111</v>
-      </c>
       <c r="E31" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G31" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -3604,19 +3589,19 @@
         <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D32" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E32" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G32" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -3627,19 +3612,19 @@
         <v>31</v>
       </c>
       <c r="C33" t="s">
+        <v>112</v>
+      </c>
+      <c r="E33" t="s">
+        <v>173</v>
+      </c>
+      <c r="F33" t="s">
         <v>113</v>
       </c>
-      <c r="E33" t="s">
-        <v>174</v>
-      </c>
-      <c r="F33" t="s">
-        <v>114</v>
-      </c>
       <c r="G33" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -3650,19 +3635,19 @@
         <v>32</v>
       </c>
       <c r="C34" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E34" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F34" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G34" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -3673,19 +3658,19 @@
         <v>33</v>
       </c>
       <c r="C35" t="s">
+        <v>115</v>
+      </c>
+      <c r="E35" t="s">
+        <v>174</v>
+      </c>
+      <c r="F35" t="s">
         <v>116</v>
       </c>
-      <c r="E35" t="s">
-        <v>175</v>
-      </c>
-      <c r="F35" t="s">
-        <v>117</v>
-      </c>
       <c r="G35" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -3696,19 +3681,19 @@
         <v>34</v>
       </c>
       <c r="C36" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E36" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F36" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G36" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -3719,19 +3704,19 @@
         <v>35</v>
       </c>
       <c r="C37" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E37" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F37" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G37" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -3742,19 +3727,19 @@
         <v>36</v>
       </c>
       <c r="C38" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E38" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F38" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G38" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -3765,19 +3750,19 @@
         <v>37</v>
       </c>
       <c r="C39" t="s">
+        <v>120</v>
+      </c>
+      <c r="E39" t="s">
+        <v>175</v>
+      </c>
+      <c r="F39" t="s">
         <v>121</v>
       </c>
-      <c r="E39" t="s">
-        <v>176</v>
-      </c>
-      <c r="F39" t="s">
-        <v>122</v>
-      </c>
       <c r="G39" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -3788,16 +3773,16 @@
         <v>38</v>
       </c>
       <c r="C40" t="s">
+        <v>122</v>
+      </c>
+      <c r="D40" t="s">
         <v>123</v>
       </c>
-      <c r="D40" t="s">
-        <v>124</v>
-      </c>
       <c r="E40" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G40" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H40" s="3"/>
     </row>
@@ -3809,16 +3794,16 @@
         <v>39</v>
       </c>
       <c r="C41" t="s">
+        <v>124</v>
+      </c>
+      <c r="D41" t="s">
         <v>125</v>
       </c>
-      <c r="D41" t="s">
-        <v>126</v>
-      </c>
       <c r="E41" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G41" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H41" s="3"/>
     </row>
@@ -3830,16 +3815,16 @@
         <v>40</v>
       </c>
       <c r="C42" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D42" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E42" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G42" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H42" s="3"/>
     </row>
@@ -3851,13 +3836,13 @@
         <v>41</v>
       </c>
       <c r="C43" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E43" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G43" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H43" s="3"/>
     </row>
@@ -3869,19 +3854,19 @@
         <v>42</v>
       </c>
       <c r="C44" t="s">
+        <v>128</v>
+      </c>
+      <c r="E44" t="s">
+        <v>176</v>
+      </c>
+      <c r="F44" t="s">
         <v>129</v>
       </c>
-      <c r="E44" t="s">
-        <v>177</v>
-      </c>
-      <c r="F44" t="s">
-        <v>130</v>
-      </c>
       <c r="G44" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -3892,19 +3877,19 @@
         <v>43</v>
       </c>
       <c r="C45" t="s">
+        <v>130</v>
+      </c>
+      <c r="E45" t="s">
+        <v>177</v>
+      </c>
+      <c r="F45" t="s">
         <v>131</v>
       </c>
-      <c r="E45" t="s">
-        <v>178</v>
-      </c>
-      <c r="F45" t="s">
-        <v>132</v>
-      </c>
       <c r="G45" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -3915,19 +3900,19 @@
         <v>44</v>
       </c>
       <c r="C46" t="s">
+        <v>132</v>
+      </c>
+      <c r="E46" t="s">
+        <v>178</v>
+      </c>
+      <c r="F46" t="s">
         <v>133</v>
       </c>
-      <c r="E46" t="s">
-        <v>179</v>
-      </c>
-      <c r="F46" t="s">
-        <v>134</v>
-      </c>
       <c r="G46" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -3938,19 +3923,19 @@
         <v>45</v>
       </c>
       <c r="C47" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E47" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F47" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G47" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -3961,19 +3946,19 @@
         <v>46</v>
       </c>
       <c r="C48" t="s">
+        <v>135</v>
+      </c>
+      <c r="E48" t="s">
+        <v>179</v>
+      </c>
+      <c r="F48" t="s">
         <v>136</v>
       </c>
-      <c r="E48" t="s">
-        <v>180</v>
-      </c>
-      <c r="F48" t="s">
-        <v>137</v>
-      </c>
       <c r="G48" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -3984,19 +3969,19 @@
         <v>47</v>
       </c>
       <c r="C49" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E49" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F49" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G49" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -4007,19 +3992,19 @@
         <v>48</v>
       </c>
       <c r="C50" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E50" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F50" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G50" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -4030,16 +4015,16 @@
         <v>49</v>
       </c>
       <c r="C51" t="s">
+        <v>139</v>
+      </c>
+      <c r="F51" t="s">
         <v>140</v>
       </c>
-      <c r="F51" t="s">
-        <v>141</v>
-      </c>
       <c r="G51" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -4050,19 +4035,19 @@
         <v>50</v>
       </c>
       <c r="C52" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E52" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F52" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G52" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -4073,19 +4058,19 @@
         <v>51</v>
       </c>
       <c r="C53" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E53" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F53" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G53" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -4096,19 +4081,19 @@
         <v>52</v>
       </c>
       <c r="C54" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E54" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F54" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G54" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -4119,19 +4104,19 @@
         <v>53</v>
       </c>
       <c r="C55" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E55" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F55" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G55" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -4142,16 +4127,16 @@
         <v>54</v>
       </c>
       <c r="C56" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D56" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E56" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G56" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H56" s="3"/>
     </row>
@@ -4163,13 +4148,13 @@
         <v>55</v>
       </c>
       <c r="C57" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E57" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G57" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H57" s="3"/>
     </row>
@@ -4181,16 +4166,16 @@
         <v>56</v>
       </c>
       <c r="C58" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D58" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E58" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G58" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H58" s="3"/>
     </row>
@@ -4202,13 +4187,13 @@
         <v>57</v>
       </c>
       <c r="C59" t="s">
+        <v>148</v>
+      </c>
+      <c r="E59" t="s">
+        <v>180</v>
+      </c>
+      <c r="F59" t="s">
         <v>149</v>
-      </c>
-      <c r="E59" t="s">
-        <v>181</v>
-      </c>
-      <c r="F59" t="s">
-        <v>150</v>
       </c>
       <c r="H59" s="3"/>
     </row>
@@ -4220,13 +4205,13 @@
         <v>58</v>
       </c>
       <c r="C60" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E60" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F60" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H60" s="3"/>
     </row>
@@ -4238,13 +4223,13 @@
         <v>59</v>
       </c>
       <c r="C61" t="s">
+        <v>148</v>
+      </c>
+      <c r="E61" t="s">
+        <v>180</v>
+      </c>
+      <c r="F61" t="s">
         <v>149</v>
-      </c>
-      <c r="E61" t="s">
-        <v>181</v>
-      </c>
-      <c r="F61" t="s">
-        <v>150</v>
       </c>
       <c r="H61" s="3"/>
     </row>
@@ -4256,13 +4241,13 @@
         <v>60</v>
       </c>
       <c r="C62" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E62" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F62" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H62" s="3"/>
     </row>
@@ -4274,13 +4259,13 @@
         <v>61</v>
       </c>
       <c r="C63" t="s">
+        <v>148</v>
+      </c>
+      <c r="E63" t="s">
+        <v>180</v>
+      </c>
+      <c r="F63" t="s">
         <v>149</v>
-      </c>
-      <c r="E63" t="s">
-        <v>181</v>
-      </c>
-      <c r="F63" t="s">
-        <v>150</v>
       </c>
       <c r="H63" s="3"/>
     </row>
@@ -4292,13 +4277,13 @@
         <v>62</v>
       </c>
       <c r="C64" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E64" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F64" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H64" s="3"/>
     </row>
@@ -4310,13 +4295,13 @@
         <v>63</v>
       </c>
       <c r="C65" t="s">
+        <v>148</v>
+      </c>
+      <c r="E65" t="s">
+        <v>180</v>
+      </c>
+      <c r="F65" t="s">
         <v>149</v>
-      </c>
-      <c r="E65" t="s">
-        <v>181</v>
-      </c>
-      <c r="F65" t="s">
-        <v>150</v>
       </c>
       <c r="H65" s="3"/>
     </row>
@@ -4328,13 +4313,13 @@
         <v>64</v>
       </c>
       <c r="C66" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E66" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F66" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H66" s="3"/>
     </row>
@@ -4346,13 +4331,13 @@
         <v>65</v>
       </c>
       <c r="C67" t="s">
+        <v>148</v>
+      </c>
+      <c r="E67" t="s">
+        <v>180</v>
+      </c>
+      <c r="F67" t="s">
         <v>149</v>
-      </c>
-      <c r="E67" t="s">
-        <v>181</v>
-      </c>
-      <c r="F67" t="s">
-        <v>150</v>
       </c>
       <c r="H67" s="3"/>
     </row>
@@ -4364,13 +4349,13 @@
         <v>66</v>
       </c>
       <c r="C68" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E68" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F68" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H68" s="3"/>
     </row>
@@ -4382,13 +4367,13 @@
         <v>67</v>
       </c>
       <c r="C69" t="s">
+        <v>148</v>
+      </c>
+      <c r="E69" t="s">
+        <v>180</v>
+      </c>
+      <c r="F69" t="s">
         <v>149</v>
-      </c>
-      <c r="E69" t="s">
-        <v>181</v>
-      </c>
-      <c r="F69" t="s">
-        <v>150</v>
       </c>
       <c r="H69" s="3"/>
     </row>
@@ -4400,13 +4385,13 @@
         <v>68</v>
       </c>
       <c r="C70" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E70" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F70" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H70" s="3"/>
     </row>
@@ -4418,13 +4403,13 @@
         <v>69</v>
       </c>
       <c r="C71" t="s">
+        <v>148</v>
+      </c>
+      <c r="E71" t="s">
+        <v>180</v>
+      </c>
+      <c r="F71" t="s">
         <v>149</v>
-      </c>
-      <c r="E71" t="s">
-        <v>181</v>
-      </c>
-      <c r="F71" t="s">
-        <v>150</v>
       </c>
       <c r="H71" s="3"/>
     </row>
@@ -4436,13 +4421,13 @@
         <v>70</v>
       </c>
       <c r="C72" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E72" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F72" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H72" s="3"/>
     </row>
@@ -4454,13 +4439,13 @@
         <v>71</v>
       </c>
       <c r="C73" t="s">
+        <v>148</v>
+      </c>
+      <c r="E73" t="s">
+        <v>180</v>
+      </c>
+      <c r="F73" t="s">
         <v>149</v>
-      </c>
-      <c r="E73" t="s">
-        <v>181</v>
-      </c>
-      <c r="F73" t="s">
-        <v>150</v>
       </c>
       <c r="H73" s="3"/>
     </row>
@@ -4472,13 +4457,13 @@
         <v>72</v>
       </c>
       <c r="C74" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E74" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F74" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H74" s="3"/>
     </row>
@@ -4490,16 +4475,16 @@
         <v>73</v>
       </c>
       <c r="C75" t="s">
+        <v>158</v>
+      </c>
+      <c r="E75" t="s">
+        <v>169</v>
+      </c>
+      <c r="F75" t="s">
         <v>159</v>
       </c>
-      <c r="E75" t="s">
-        <v>170</v>
-      </c>
-      <c r="F75" t="s">
-        <v>160</v>
-      </c>
       <c r="H75" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -4510,16 +4495,16 @@
         <v>74</v>
       </c>
       <c r="C76" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E76" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F76" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H76" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -4530,16 +4515,16 @@
         <v>75</v>
       </c>
       <c r="C77" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E77" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F77" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H77" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -4550,16 +4535,16 @@
         <v>76</v>
       </c>
       <c r="C78" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E78" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F78" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H78" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -4570,16 +4555,16 @@
         <v>77</v>
       </c>
       <c r="C79" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E79" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F79" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H79" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -4587,19 +4572,19 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
+        <v>164</v>
+      </c>
+      <c r="C80" t="s">
         <v>165</v>
       </c>
-      <c r="C80" t="s">
-        <v>166</v>
-      </c>
       <c r="E80" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F80" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -4610,16 +4595,16 @@
         <v>79</v>
       </c>
       <c r="C81" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E81" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F81" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H81" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Version 0.2.10: Bug fix #14. New plugin: SUEWSAnalyzer. General Bug fixing
</commit_message>
<xml_diff>
--- a/SUEWSPrepare/Input/SUEWS_SiteSelect.xlsx
+++ b/SUEWSPrepare/Input/SUEWS_SiteSelect.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="345" windowWidth="18690" windowHeight="8835" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="345" windowWidth="18690" windowHeight="8835"/>
   </bookViews>
   <sheets>
     <sheet name="SUEWS_SiteSelect" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="237">
   <si>
     <t>Grid</t>
   </si>
@@ -590,6 +590,9 @@
     <t>Evergreen</t>
   </si>
   <si>
+    <t>Decidious</t>
+  </si>
+  <si>
     <t>Grass</t>
   </si>
   <si>
@@ -716,10 +719,16 @@
     <t>Reference</t>
   </si>
   <si>
-    <t>Kotthaus and Grimmond (2013, 2014a, 2014b)</t>
-  </si>
-  <si>
-    <t>Deciduous</t>
+    <t>TrafficRate</t>
+  </si>
+  <si>
+    <t>BuildEnergyUse</t>
+  </si>
+  <si>
+    <t>ActivityProfWD</t>
+  </si>
+  <si>
+    <t>ActivityProfWE</t>
   </si>
 </sst>
 </file>
@@ -1564,11 +1573,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CV83"/>
+  <dimension ref="A1:CZ78"/>
   <sheetViews>
-    <sheetView topLeftCell="CB1" workbookViewId="0">
-      <selection activeCell="CC7" sqref="CC7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1577,7 +1584,7 @@
     <col min="41" max="41" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -1869,8 +1876,20 @@
       <c r="CS1">
         <v>97</v>
       </c>
-    </row>
-    <row r="2" spans="1:100" x14ac:dyDescent="0.25">
+      <c r="CT1">
+        <v>98</v>
+      </c>
+      <c r="CU1">
+        <v>99</v>
+      </c>
+      <c r="CV1">
+        <v>100</v>
+      </c>
+      <c r="CW1">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1965,219 +1984,231 @@
         <v>30</v>
       </c>
       <c r="AF2" t="s">
+        <v>233</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>234</v>
+      </c>
+      <c r="AH2" t="s">
         <v>31</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AI2" t="s">
         <v>32</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AJ2" t="s">
         <v>33</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AK2" t="s">
         <v>34</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AL2" t="s">
         <v>35</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AM2" t="s">
         <v>36</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AN2" t="s">
         <v>37</v>
       </c>
-      <c r="AM2" t="s">
+      <c r="AO2" t="s">
         <v>38</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AP2" t="s">
         <v>39</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AQ2" t="s">
         <v>40</v>
       </c>
-      <c r="AP2" t="s">
+      <c r="AR2" t="s">
         <v>41</v>
       </c>
-      <c r="AQ2" t="s">
+      <c r="AS2" t="s">
         <v>42</v>
       </c>
-      <c r="AR2" t="s">
+      <c r="AT2" t="s">
         <v>43</v>
       </c>
-      <c r="AS2" t="s">
+      <c r="AU2" t="s">
         <v>44</v>
       </c>
-      <c r="AT2" t="s">
+      <c r="AV2" t="s">
         <v>45</v>
       </c>
-      <c r="AU2" t="s">
+      <c r="AW2" t="s">
         <v>46</v>
       </c>
-      <c r="AV2" t="s">
+      <c r="AX2" t="s">
         <v>47</v>
       </c>
-      <c r="AW2" t="s">
+      <c r="AY2" t="s">
         <v>48</v>
       </c>
-      <c r="AX2" t="s">
+      <c r="AZ2" t="s">
+        <v>235</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>236</v>
+      </c>
+      <c r="BB2" t="s">
         <v>49</v>
       </c>
-      <c r="AY2" t="s">
+      <c r="BC2" t="s">
         <v>50</v>
       </c>
-      <c r="AZ2" t="s">
+      <c r="BD2" t="s">
         <v>51</v>
       </c>
-      <c r="BA2" t="s">
+      <c r="BE2" t="s">
         <v>52</v>
       </c>
-      <c r="BB2" t="s">
+      <c r="BF2" t="s">
         <v>53</v>
       </c>
-      <c r="BC2" t="s">
+      <c r="BG2" t="s">
         <v>54</v>
       </c>
-      <c r="BD2" t="s">
+      <c r="BH2" t="s">
         <v>55</v>
       </c>
-      <c r="BE2" t="s">
+      <c r="BI2" t="s">
         <v>56</v>
       </c>
-      <c r="BF2" t="s">
+      <c r="BJ2" t="s">
         <v>57</v>
       </c>
-      <c r="BG2" t="s">
+      <c r="BK2" t="s">
         <v>58</v>
       </c>
-      <c r="BH2" t="s">
+      <c r="BL2" t="s">
         <v>59</v>
       </c>
-      <c r="BI2" t="s">
+      <c r="BM2" t="s">
         <v>60</v>
       </c>
-      <c r="BJ2" t="s">
+      <c r="BN2" t="s">
         <v>61</v>
       </c>
-      <c r="BK2" t="s">
+      <c r="BO2" t="s">
         <v>62</v>
       </c>
-      <c r="BL2" t="s">
+      <c r="BP2" t="s">
         <v>63</v>
       </c>
-      <c r="BM2" t="s">
+      <c r="BQ2" t="s">
         <v>64</v>
       </c>
-      <c r="BN2" t="s">
+      <c r="BR2" t="s">
         <v>65</v>
       </c>
-      <c r="BO2" t="s">
+      <c r="BS2" t="s">
         <v>66</v>
       </c>
-      <c r="BP2" t="s">
+      <c r="BT2" t="s">
         <v>67</v>
       </c>
-      <c r="BQ2" t="s">
+      <c r="BU2" t="s">
         <v>68</v>
       </c>
-      <c r="BR2" t="s">
+      <c r="BV2" t="s">
         <v>69</v>
       </c>
-      <c r="BS2" t="s">
+      <c r="BW2" t="s">
         <v>70</v>
       </c>
-      <c r="BT2" t="s">
+      <c r="BX2" t="s">
         <v>71</v>
       </c>
-      <c r="BU2" t="s">
+      <c r="BY2" t="s">
         <v>72</v>
       </c>
-      <c r="BV2" t="s">
+      <c r="BZ2" t="s">
         <v>73</v>
       </c>
-      <c r="BW2" t="s">
+      <c r="CA2" t="s">
         <v>74</v>
       </c>
-      <c r="BX2" t="s">
+      <c r="CB2" t="s">
         <v>75</v>
       </c>
-      <c r="BY2" t="s">
+      <c r="CC2" t="s">
         <v>76</v>
       </c>
-      <c r="BZ2" t="s">
+      <c r="CD2" t="s">
         <v>77</v>
       </c>
-      <c r="CA2" t="s">
+      <c r="CE2" t="s">
         <v>78</v>
       </c>
-      <c r="CB2" t="s">
+      <c r="CF2" t="s">
         <v>79</v>
       </c>
-      <c r="CC2" t="s">
-        <v>213</v>
-      </c>
-      <c r="CD2" t="s">
+      <c r="CG2" t="s">
         <v>214</v>
       </c>
-      <c r="CE2" t="s">
+      <c r="CH2" t="s">
         <v>215</v>
       </c>
-      <c r="CF2" t="s">
+      <c r="CI2" t="s">
         <v>216</v>
       </c>
-      <c r="CG2" t="s">
+      <c r="CJ2" t="s">
         <v>217</v>
       </c>
-      <c r="CH2" t="s">
+      <c r="CK2" t="s">
         <v>218</v>
       </c>
-      <c r="CI2" t="s">
+      <c r="CL2" t="s">
         <v>219</v>
       </c>
-      <c r="CJ2" t="s">
+      <c r="CM2" t="s">
         <v>220</v>
       </c>
-      <c r="CK2" t="s">
+      <c r="CN2" t="s">
         <v>221</v>
       </c>
-      <c r="CL2" t="s">
+      <c r="CO2" t="s">
         <v>222</v>
       </c>
-      <c r="CM2" t="s">
+      <c r="CP2" t="s">
         <v>223</v>
       </c>
-      <c r="CN2" t="s">
+      <c r="CQ2" t="s">
         <v>224</v>
       </c>
-      <c r="CO2" t="s">
+      <c r="CR2" t="s">
         <v>225</v>
       </c>
-      <c r="CP2" t="s">
+      <c r="CS2" t="s">
         <v>226</v>
       </c>
-      <c r="CQ2" t="s">
+      <c r="CT2" t="s">
         <v>227</v>
       </c>
-      <c r="CR2" t="s">
+      <c r="CU2" t="s">
         <v>228</v>
       </c>
-      <c r="CS2" t="s">
+      <c r="CV2" t="s">
         <v>229</v>
       </c>
-      <c r="CT2" t="s">
-        <v>80</v>
-      </c>
-      <c r="CU2" t="s">
+      <c r="CW2" t="s">
         <v>230</v>
       </c>
-      <c r="CV2" t="s">
+      <c r="CX2" t="s">
+        <v>80</v>
+      </c>
+      <c r="CY2" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="3" spans="1:100" x14ac:dyDescent="0.25">
+      <c r="CZ2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="3" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>2012</v>
+        <v>2015</v>
       </c>
       <c r="C3">
         <v>85</v>
@@ -2186,16 +2217,16 @@
         <v>302</v>
       </c>
       <c r="E3">
-        <v>51.51</v>
+        <v>51.284399639999997</v>
       </c>
       <c r="F3">
-        <v>0.12</v>
+        <v>0.108141738</v>
       </c>
       <c r="G3">
-        <v>2221.56</v>
+        <v>1</v>
       </c>
       <c r="H3">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -2207,25 +2238,25 @@
         <v>0</v>
       </c>
       <c r="L3">
-        <v>0.43</v>
+        <v>0.58099999999999996</v>
       </c>
       <c r="M3">
-        <v>0.38</v>
+        <v>0</v>
       </c>
       <c r="N3">
         <v>0</v>
       </c>
       <c r="O3">
-        <v>0.02</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="P3">
-        <v>0.03</v>
+        <v>0.41099999999999998</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>0.14000000000000001</v>
+        <v>0</v>
       </c>
       <c r="S3">
         <v>0</v>
@@ -2237,124 +2268,124 @@
         <v>0</v>
       </c>
       <c r="V3">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="W3">
-        <v>22</v>
+        <v>3.0960000000000001</v>
       </c>
       <c r="X3">
-        <v>22</v>
+        <v>3.0960000000000001</v>
       </c>
       <c r="Y3">
-        <v>1.9</v>
+        <v>0</v>
       </c>
       <c r="Z3">
-        <v>14.2</v>
+        <v>0</v>
       </c>
       <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3">
+        <v>2.4E-2</v>
+      </c>
+      <c r="AC3">
+        <v>2.4E-2</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <v>0</v>
+      </c>
+      <c r="AF3">
         <v>-999</v>
       </c>
-      <c r="AB3">
+      <c r="AG3">
         <v>-999</v>
       </c>
-      <c r="AC3">
-        <v>-999</v>
-      </c>
-      <c r="AD3">
-        <v>310.39999999999998</v>
-      </c>
-      <c r="AE3">
-        <v>204.6</v>
-      </c>
-      <c r="AF3">
-        <v>551</v>
-      </c>
-      <c r="AG3">
-        <v>552</v>
-      </c>
       <c r="AH3">
-        <v>551</v>
+        <v>661</v>
       </c>
       <c r="AI3">
-        <v>552</v>
+        <v>662</v>
       </c>
       <c r="AJ3">
-        <v>553</v>
+        <v>700</v>
       </c>
       <c r="AK3">
-        <v>553</v>
+        <v>701</v>
       </c>
       <c r="AL3">
-        <v>551</v>
+        <v>702</v>
       </c>
       <c r="AM3">
+        <v>703</v>
+      </c>
+      <c r="AN3">
+        <v>661</v>
+      </c>
+      <c r="AO3">
         <v>0.25</v>
-      </c>
-      <c r="AN3">
-        <v>1</v>
-      </c>
-      <c r="AO3">
-        <v>10</v>
       </c>
       <c r="AP3">
         <v>1</v>
       </c>
       <c r="AQ3">
+        <v>10</v>
+      </c>
+      <c r="AR3">
+        <v>1</v>
+      </c>
+      <c r="AS3">
         <v>100</v>
-      </c>
-      <c r="AR3">
-        <v>660</v>
-      </c>
-      <c r="AS3">
-        <v>660</v>
       </c>
       <c r="AT3">
         <v>660</v>
       </c>
       <c r="AU3">
-        <v>551</v>
+        <v>660</v>
       </c>
       <c r="AV3">
-        <v>551</v>
+        <v>660</v>
       </c>
       <c r="AW3">
-        <v>552</v>
+        <v>661</v>
       </c>
       <c r="AX3">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="AY3">
-        <v>660</v>
+        <v>662</v>
       </c>
       <c r="AZ3">
-        <v>660</v>
+        <v>55663</v>
       </c>
       <c r="BA3">
-        <v>660</v>
+        <v>55664</v>
       </c>
       <c r="BB3">
         <v>660</v>
       </c>
       <c r="BC3">
-        <v>0</v>
+        <v>660</v>
       </c>
       <c r="BD3">
-        <v>0.1</v>
+        <v>660</v>
       </c>
       <c r="BE3">
-        <v>100</v>
+        <v>660</v>
       </c>
       <c r="BF3">
-        <v>0</v>
+        <v>660</v>
       </c>
       <c r="BG3">
         <v>0</v>
       </c>
       <c r="BH3">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="BI3">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="BJ3">
         <v>0</v>
@@ -2393,143 +2424,157 @@
         <v>0</v>
       </c>
       <c r="BV3">
-        <v>551</v>
+        <v>0</v>
       </c>
       <c r="BW3">
-        <v>552</v>
+        <v>0</v>
       </c>
       <c r="BX3">
-        <v>553</v>
+        <v>0</v>
       </c>
       <c r="BY3">
-        <v>554</v>
+        <v>0</v>
       </c>
       <c r="BZ3">
-        <v>555</v>
+        <v>661</v>
       </c>
       <c r="CA3">
-        <v>556</v>
+        <v>662</v>
       </c>
       <c r="CB3">
-        <v>557</v>
+        <v>663</v>
       </c>
       <c r="CC3">
-        <v>950000</v>
+        <v>664</v>
       </c>
       <c r="CD3">
-        <v>0.15</v>
+        <v>665</v>
       </c>
       <c r="CE3">
-        <v>0.05</v>
+        <v>666</v>
       </c>
       <c r="CF3">
-        <v>0.8</v>
+        <v>667</v>
       </c>
       <c r="CG3">
+        <v>0</v>
+      </c>
+      <c r="CH3">
+        <v>1</v>
+      </c>
+      <c r="CI3">
+        <v>0</v>
+      </c>
+      <c r="CJ3">
+        <v>0</v>
+      </c>
+      <c r="CK3">
         <v>806</v>
       </c>
-      <c r="CH3">
+      <c r="CL3">
         <v>807</v>
       </c>
-      <c r="CI3">
+      <c r="CM3">
         <v>808</v>
       </c>
-      <c r="CJ3">
-        <v>0.15</v>
-      </c>
-      <c r="CK3">
-        <v>0.45</v>
-      </c>
-      <c r="CL3">
-        <v>0.05</v>
-      </c>
-      <c r="CM3">
-        <v>0.1</v>
-      </c>
       <c r="CN3">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="CO3">
+        <v>0</v>
+      </c>
+      <c r="CP3">
+        <v>1</v>
+      </c>
+      <c r="CQ3">
+        <v>0</v>
+      </c>
+      <c r="CR3">
+        <v>0</v>
+      </c>
+      <c r="CS3">
         <v>801</v>
       </c>
-      <c r="CP3">
-        <v>802</v>
-      </c>
-      <c r="CQ3">
+      <c r="CT3">
         <v>803</v>
       </c>
-      <c r="CR3">
-        <v>804</v>
-      </c>
-      <c r="CS3">
-        <v>805</v>
-      </c>
-      <c r="CT3" t="s">
-        <v>80</v>
-      </c>
-      <c r="CU3" t="s">
+      <c r="CU3">
+        <v>8021</v>
+      </c>
+      <c r="CV3">
+        <v>8022</v>
+      </c>
+      <c r="CW3">
+        <v>8041</v>
+      </c>
+      <c r="CX3" t="s">
+        <v>80</v>
+      </c>
+      <c r="CY3" t="s">
         <v>81</v>
       </c>
-      <c r="CV3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="4" spans="1:100" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>-9</v>
       </c>
     </row>
-    <row r="5" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>-9</v>
       </c>
     </row>
-    <row r="7" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:104" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>80</v>
       </c>
@@ -2841,31 +2886,6 @@
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2879,8 +2899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="54" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2898,28 +2918,28 @@
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>206</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2936,7 +2956,7 @@
         <v>83</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="G2" t="s">
         <v>185</v>
@@ -2945,7 +2965,7 @@
         <v>182</v>
       </c>
       <c r="I2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -3040,7 +3060,7 @@
         <v>182</v>
       </c>
       <c r="I6" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
@@ -3066,7 +3086,7 @@
         <v>182</v>
       </c>
       <c r="I7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -3092,7 +3112,7 @@
         <v>182</v>
       </c>
       <c r="I8" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -3112,7 +3132,7 @@
         <v>167</v>
       </c>
       <c r="F9" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="G9" t="s">
         <v>185</v>
@@ -3467,7 +3487,7 @@
         <v>170</v>
       </c>
       <c r="F26" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="G26" t="s">
         <v>185</v>
@@ -3491,7 +3511,7 @@
         <v>170</v>
       </c>
       <c r="F27" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="G27" t="s">
         <v>185</v>
@@ -3693,7 +3713,7 @@
         <v>185</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>233</v>
+        <v>190</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -3716,7 +3736,7 @@
         <v>185</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -3739,7 +3759,7 @@
         <v>185</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -3762,7 +3782,7 @@
         <v>185</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -3866,7 +3886,7 @@
         <v>185</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -3889,7 +3909,7 @@
         <v>185</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -3912,7 +3932,7 @@
         <v>185</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -3935,7 +3955,7 @@
         <v>185</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -3958,7 +3978,7 @@
         <v>185</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -3981,7 +4001,7 @@
         <v>185</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -4004,7 +4024,7 @@
         <v>185</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -4024,7 +4044,7 @@
         <v>185</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -4047,7 +4067,7 @@
         <v>185</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -4070,7 +4090,7 @@
         <v>185</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -4093,7 +4113,7 @@
         <v>185</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -4116,7 +4136,7 @@
         <v>185</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -4544,7 +4564,7 @@
         <v>159</v>
       </c>
       <c r="H78" s="3" t="s">
-        <v>233</v>
+        <v>190</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -4564,7 +4584,7 @@
         <v>159</v>
       </c>
       <c r="H79" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -4584,7 +4604,7 @@
         <v>159</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -4604,7 +4624,7 @@
         <v>159</v>
       </c>
       <c r="H81" s="3" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Version 0.2.11: Major changes to SUEWS-related plugins to prepare for new model version. Bug fixing
</commit_message>
<xml_diff>
--- a/SUEWSPrepare/Input/SUEWS_SiteSelect.xlsx
+++ b/SUEWSPrepare/Input/SUEWS_SiteSelect.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="240">
   <si>
     <t>Grid</t>
   </si>
@@ -729,6 +729,15 @@
   </si>
   <si>
     <t>ActivityProfWE</t>
+  </si>
+  <si>
+    <t>Timezone</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>Kotthaus and Grimmond (2013, 2014a, 2014b)</t>
   </si>
 </sst>
 </file>
@@ -1573,9 +1582,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CZ78"/>
+  <dimension ref="A1:DB73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1584,7 +1595,7 @@
     <col min="41" max="41" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:104" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -1888,8 +1899,14 @@
       <c r="CW1">
         <v>101</v>
       </c>
-    </row>
-    <row r="2" spans="1:104" x14ac:dyDescent="0.25">
+      <c r="CX1">
+        <v>102</v>
+      </c>
+      <c r="CY1">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1909,306 +1926,312 @@
         <v>5</v>
       </c>
       <c r="G2" t="s">
+        <v>237</v>
+      </c>
+      <c r="H2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>7</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
+        <v>238</v>
+      </c>
+      <c r="K2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>9</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>10</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>11</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>12</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>13</v>
       </c>
-      <c r="O2" t="s">
+      <c r="Q2" t="s">
         <v>14</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="S2" t="s">
         <v>16</v>
       </c>
-      <c r="R2" t="s">
+      <c r="T2" t="s">
         <v>17</v>
       </c>
-      <c r="S2" t="s">
+      <c r="U2" t="s">
         <v>18</v>
       </c>
-      <c r="T2" t="s">
+      <c r="V2" t="s">
         <v>19</v>
       </c>
-      <c r="U2" t="s">
+      <c r="W2" t="s">
         <v>20</v>
       </c>
-      <c r="V2" t="s">
+      <c r="X2" t="s">
         <v>21</v>
       </c>
-      <c r="W2" t="s">
+      <c r="Y2" t="s">
         <v>22</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Z2" t="s">
         <v>23</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="AA2" t="s">
         <v>24</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AB2" t="s">
         <v>25</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AC2" t="s">
         <v>26</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AD2" t="s">
         <v>27</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AE2" t="s">
         <v>28</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AF2" t="s">
         <v>29</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AG2" t="s">
         <v>30</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AH2" t="s">
         <v>233</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AI2" t="s">
         <v>234</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AJ2" t="s">
         <v>31</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AK2" t="s">
         <v>32</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AL2" t="s">
         <v>33</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AM2" t="s">
         <v>34</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AN2" t="s">
         <v>35</v>
       </c>
-      <c r="AM2" t="s">
+      <c r="AO2" t="s">
         <v>36</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AP2" t="s">
         <v>37</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AQ2" t="s">
         <v>38</v>
       </c>
-      <c r="AP2" t="s">
+      <c r="AR2" t="s">
         <v>39</v>
       </c>
-      <c r="AQ2" t="s">
+      <c r="AS2" t="s">
         <v>40</v>
       </c>
-      <c r="AR2" t="s">
+      <c r="AT2" t="s">
         <v>41</v>
       </c>
-      <c r="AS2" t="s">
+      <c r="AU2" t="s">
         <v>42</v>
       </c>
-      <c r="AT2" t="s">
+      <c r="AV2" t="s">
         <v>43</v>
       </c>
-      <c r="AU2" t="s">
+      <c r="AW2" t="s">
         <v>44</v>
       </c>
-      <c r="AV2" t="s">
+      <c r="AX2" t="s">
         <v>45</v>
       </c>
-      <c r="AW2" t="s">
+      <c r="AY2" t="s">
         <v>46</v>
       </c>
-      <c r="AX2" t="s">
+      <c r="AZ2" t="s">
         <v>47</v>
       </c>
-      <c r="AY2" t="s">
+      <c r="BA2" t="s">
         <v>48</v>
       </c>
-      <c r="AZ2" t="s">
+      <c r="BB2" t="s">
         <v>235</v>
       </c>
-      <c r="BA2" t="s">
+      <c r="BC2" t="s">
         <v>236</v>
       </c>
-      <c r="BB2" t="s">
+      <c r="BD2" t="s">
         <v>49</v>
       </c>
-      <c r="BC2" t="s">
+      <c r="BE2" t="s">
         <v>50</v>
       </c>
-      <c r="BD2" t="s">
+      <c r="BF2" t="s">
         <v>51</v>
       </c>
-      <c r="BE2" t="s">
+      <c r="BG2" t="s">
         <v>52</v>
       </c>
-      <c r="BF2" t="s">
+      <c r="BH2" t="s">
         <v>53</v>
       </c>
-      <c r="BG2" t="s">
+      <c r="BI2" t="s">
         <v>54</v>
       </c>
-      <c r="BH2" t="s">
+      <c r="BJ2" t="s">
         <v>55</v>
       </c>
-      <c r="BI2" t="s">
+      <c r="BK2" t="s">
         <v>56</v>
       </c>
-      <c r="BJ2" t="s">
+      <c r="BL2" t="s">
         <v>57</v>
       </c>
-      <c r="BK2" t="s">
+      <c r="BM2" t="s">
         <v>58</v>
       </c>
-      <c r="BL2" t="s">
+      <c r="BN2" t="s">
         <v>59</v>
       </c>
-      <c r="BM2" t="s">
+      <c r="BO2" t="s">
         <v>60</v>
       </c>
-      <c r="BN2" t="s">
+      <c r="BP2" t="s">
         <v>61</v>
       </c>
-      <c r="BO2" t="s">
+      <c r="BQ2" t="s">
         <v>62</v>
       </c>
-      <c r="BP2" t="s">
+      <c r="BR2" t="s">
         <v>63</v>
       </c>
-      <c r="BQ2" t="s">
+      <c r="BS2" t="s">
         <v>64</v>
       </c>
-      <c r="BR2" t="s">
+      <c r="BT2" t="s">
         <v>65</v>
       </c>
-      <c r="BS2" t="s">
+      <c r="BU2" t="s">
         <v>66</v>
       </c>
-      <c r="BT2" t="s">
+      <c r="BV2" t="s">
         <v>67</v>
       </c>
-      <c r="BU2" t="s">
+      <c r="BW2" t="s">
         <v>68</v>
       </c>
-      <c r="BV2" t="s">
+      <c r="BX2" t="s">
         <v>69</v>
       </c>
-      <c r="BW2" t="s">
+      <c r="BY2" t="s">
         <v>70</v>
       </c>
-      <c r="BX2" t="s">
+      <c r="BZ2" t="s">
         <v>71</v>
       </c>
-      <c r="BY2" t="s">
+      <c r="CA2" t="s">
         <v>72</v>
       </c>
-      <c r="BZ2" t="s">
+      <c r="CB2" t="s">
         <v>73</v>
       </c>
-      <c r="CA2" t="s">
+      <c r="CC2" t="s">
         <v>74</v>
       </c>
-      <c r="CB2" t="s">
+      <c r="CD2" t="s">
         <v>75</v>
       </c>
-      <c r="CC2" t="s">
+      <c r="CE2" t="s">
         <v>76</v>
       </c>
-      <c r="CD2" t="s">
+      <c r="CF2" t="s">
         <v>77</v>
       </c>
-      <c r="CE2" t="s">
+      <c r="CG2" t="s">
         <v>78</v>
       </c>
-      <c r="CF2" t="s">
+      <c r="CH2" t="s">
         <v>79</v>
       </c>
-      <c r="CG2" t="s">
+      <c r="CI2" t="s">
         <v>214</v>
       </c>
-      <c r="CH2" t="s">
+      <c r="CJ2" t="s">
         <v>215</v>
       </c>
-      <c r="CI2" t="s">
+      <c r="CK2" t="s">
         <v>216</v>
       </c>
-      <c r="CJ2" t="s">
+      <c r="CL2" t="s">
         <v>217</v>
       </c>
-      <c r="CK2" t="s">
+      <c r="CM2" t="s">
         <v>218</v>
       </c>
-      <c r="CL2" t="s">
+      <c r="CN2" t="s">
         <v>219</v>
       </c>
-      <c r="CM2" t="s">
+      <c r="CO2" t="s">
         <v>220</v>
       </c>
-      <c r="CN2" t="s">
+      <c r="CP2" t="s">
         <v>221</v>
       </c>
-      <c r="CO2" t="s">
+      <c r="CQ2" t="s">
         <v>222</v>
       </c>
-      <c r="CP2" t="s">
+      <c r="CR2" t="s">
         <v>223</v>
       </c>
-      <c r="CQ2" t="s">
+      <c r="CS2" t="s">
         <v>224</v>
       </c>
-      <c r="CR2" t="s">
+      <c r="CT2" t="s">
         <v>225</v>
       </c>
-      <c r="CS2" t="s">
+      <c r="CU2" t="s">
         <v>226</v>
       </c>
-      <c r="CT2" t="s">
+      <c r="CV2" t="s">
         <v>227</v>
       </c>
-      <c r="CU2" t="s">
+      <c r="CW2" t="s">
         <v>228</v>
       </c>
-      <c r="CV2" t="s">
+      <c r="CX2" t="s">
         <v>229</v>
       </c>
-      <c r="CW2" t="s">
+      <c r="CY2" t="s">
         <v>230</v>
       </c>
-      <c r="CX2" t="s">
-        <v>80</v>
-      </c>
-      <c r="CY2" t="s">
+      <c r="CZ2" t="s">
+        <v>80</v>
+      </c>
+      <c r="DA2" t="s">
         <v>231</v>
       </c>
-      <c r="CZ2" t="s">
+      <c r="DB2" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="3" spans="1:104" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>2015</v>
+        <v>2012</v>
       </c>
       <c r="C3">
         <v>85</v>
@@ -2217,52 +2240,52 @@
         <v>302</v>
       </c>
       <c r="E3">
-        <v>51.284399639999997</v>
+        <v>51.51</v>
       </c>
       <c r="F3">
-        <v>0.108141738</v>
+        <v>0.12</v>
       </c>
       <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>2221.56</v>
+      </c>
+      <c r="I3">
+        <v>10.7</v>
+      </c>
+      <c r="J3">
+        <v>49.6</v>
+      </c>
+      <c r="K3">
         <v>1</v>
       </c>
-      <c r="H3">
+      <c r="L3">
         <v>0</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0.58099999999999996</v>
       </c>
       <c r="M3">
         <v>0</v>
       </c>
       <c r="N3">
+        <v>0.43</v>
+      </c>
+      <c r="O3">
+        <v>0.38</v>
+      </c>
+      <c r="P3">
         <v>0</v>
       </c>
-      <c r="O3">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="P3">
-        <v>0.41099999999999998</v>
-      </c>
       <c r="Q3">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="R3">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="S3">
         <v>0</v>
       </c>
       <c r="T3">
-        <v>0</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -2271,127 +2294,127 @@
         <v>0</v>
       </c>
       <c r="W3">
-        <v>3.0960000000000001</v>
+        <v>0</v>
       </c>
       <c r="X3">
-        <v>3.0960000000000001</v>
+        <v>22</v>
       </c>
       <c r="Y3">
-        <v>0</v>
+        <v>13.1</v>
       </c>
       <c r="Z3">
-        <v>0</v>
+        <v>13.1</v>
       </c>
       <c r="AA3">
-        <v>0</v>
+        <v>1.9</v>
       </c>
       <c r="AB3">
-        <v>2.4E-2</v>
+        <v>14.2</v>
       </c>
       <c r="AC3">
-        <v>2.4E-2</v>
+        <v>-999</v>
       </c>
       <c r="AD3">
-        <v>0</v>
+        <v>-999</v>
       </c>
       <c r="AE3">
-        <v>0</v>
+        <v>-999</v>
       </c>
       <c r="AF3">
         <v>-999</v>
       </c>
       <c r="AG3">
+        <v>204.58</v>
+      </c>
+      <c r="AH3">
         <v>-999</v>
       </c>
-      <c r="AH3">
+      <c r="AI3">
+        <v>-999</v>
+      </c>
+      <c r="AJ3">
         <v>661</v>
       </c>
-      <c r="AI3">
+      <c r="AK3">
         <v>662</v>
       </c>
-      <c r="AJ3">
-        <v>700</v>
-      </c>
-      <c r="AK3">
-        <v>701</v>
-      </c>
       <c r="AL3">
-        <v>702</v>
+        <v>661</v>
       </c>
       <c r="AM3">
-        <v>703</v>
+        <v>662</v>
       </c>
       <c r="AN3">
+        <v>663</v>
+      </c>
+      <c r="AO3">
+        <v>663</v>
+      </c>
+      <c r="AP3">
         <v>661</v>
       </c>
-      <c r="AO3">
+      <c r="AQ3">
         <v>0.25</v>
-      </c>
-      <c r="AP3">
-        <v>1</v>
-      </c>
-      <c r="AQ3">
-        <v>10</v>
       </c>
       <c r="AR3">
         <v>1</v>
       </c>
       <c r="AS3">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="AT3">
-        <v>660</v>
+        <v>1</v>
       </c>
       <c r="AU3">
-        <v>660</v>
+        <v>200</v>
       </c>
       <c r="AV3">
-        <v>660</v>
+        <v>99999</v>
       </c>
       <c r="AW3">
+        <v>99999</v>
+      </c>
+      <c r="AX3">
+        <v>99999</v>
+      </c>
+      <c r="AY3">
         <v>661</v>
       </c>
-      <c r="AX3">
+      <c r="AZ3">
         <v>661</v>
       </c>
-      <c r="AY3">
+      <c r="BA3">
         <v>662</v>
       </c>
-      <c r="AZ3">
-        <v>55663</v>
-      </c>
-      <c r="BA3">
-        <v>55664</v>
-      </c>
       <c r="BB3">
-        <v>660</v>
+        <v>90000</v>
       </c>
       <c r="BC3">
-        <v>660</v>
+        <v>90000</v>
       </c>
       <c r="BD3">
-        <v>660</v>
+        <v>99999</v>
       </c>
       <c r="BE3">
-        <v>660</v>
+        <v>99999</v>
       </c>
       <c r="BF3">
-        <v>660</v>
+        <v>99999</v>
       </c>
       <c r="BG3">
+        <v>99999</v>
+      </c>
+      <c r="BH3">
+        <v>99999</v>
+      </c>
+      <c r="BI3">
         <v>0</v>
-      </c>
-      <c r="BH3">
-        <v>0.1</v>
-      </c>
-      <c r="BI3">
-        <v>100</v>
       </c>
       <c r="BJ3">
         <v>0</v>
       </c>
       <c r="BK3">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="BL3">
         <v>0</v>
@@ -2436,145 +2459,154 @@
         <v>0</v>
       </c>
       <c r="BZ3">
+        <v>0</v>
+      </c>
+      <c r="CA3">
+        <v>0</v>
+      </c>
+      <c r="CB3">
         <v>661</v>
       </c>
-      <c r="CA3">
+      <c r="CC3">
         <v>662</v>
       </c>
-      <c r="CB3">
+      <c r="CD3">
         <v>663</v>
       </c>
-      <c r="CC3">
+      <c r="CE3">
         <v>664</v>
       </c>
-      <c r="CD3">
+      <c r="CF3">
         <v>665</v>
       </c>
-      <c r="CE3">
+      <c r="CG3">
         <v>666</v>
       </c>
-      <c r="CF3">
+      <c r="CH3">
         <v>667</v>
       </c>
-      <c r="CG3">
-        <v>0</v>
-      </c>
-      <c r="CH3">
-        <v>1</v>
-      </c>
       <c r="CI3">
-        <v>0</v>
+        <v>1.08</v>
       </c>
       <c r="CJ3">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="CK3">
+        <v>0.05</v>
+      </c>
+      <c r="CL3">
+        <v>0.8</v>
+      </c>
+      <c r="CM3">
         <v>806</v>
       </c>
-      <c r="CL3">
+      <c r="CN3">
         <v>807</v>
       </c>
-      <c r="CM3">
+      <c r="CO3">
         <v>808</v>
       </c>
-      <c r="CN3">
-        <v>0</v>
-      </c>
-      <c r="CO3">
-        <v>0</v>
-      </c>
       <c r="CP3">
-        <v>1</v>
+        <v>0.15</v>
       </c>
       <c r="CQ3">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="CR3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="CS3">
+        <v>0.1</v>
+      </c>
+      <c r="CT3">
+        <v>0.25</v>
+      </c>
+      <c r="CU3">
         <v>801</v>
       </c>
-      <c r="CT3">
+      <c r="CV3">
+        <v>802</v>
+      </c>
+      <c r="CW3">
         <v>803</v>
       </c>
-      <c r="CU3">
-        <v>8021</v>
-      </c>
-      <c r="CV3">
-        <v>8022</v>
-      </c>
-      <c r="CW3">
-        <v>8041</v>
-      </c>
-      <c r="CX3" t="s">
-        <v>80</v>
-      </c>
-      <c r="CY3" t="s">
+      <c r="CX3">
+        <v>804</v>
+      </c>
+      <c r="CY3">
+        <v>805</v>
+      </c>
+      <c r="CZ3" t="s">
+        <v>80</v>
+      </c>
+      <c r="DA3" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="4" spans="1:104" x14ac:dyDescent="0.25">
+      <c r="DB3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="4" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>-9</v>
       </c>
     </row>
-    <row r="5" spans="1:104" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>-9</v>
       </c>
     </row>
-    <row r="6" spans="1:104" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:104" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:104" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:104" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:104" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:104" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:104" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:104" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:104" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:104" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:104" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>80</v>
       </c>
@@ -2861,31 +2893,6 @@
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
         <v>80</v>
       </c>
     </row>

</xml_diff>

<commit_message>
1.4.2 : Response to issue #42 and #46. Initiation of migration to QGIS3.
</commit_message>
<xml_diff>
--- a/SUEWSPrepare/Input/SUEWS_SiteSelect.xlsx
+++ b/SUEWSPrepare/Input/SUEWS_SiteSelect.xlsx
@@ -11,14 +11,14 @@
     <sheet name="Metadata" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Metadata!$H$1:$H$81</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Metadata!$H$1:$H$85</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="241">
   <si>
     <t>Grid</t>
   </si>
@@ -725,12 +725,6 @@
     <t>BuildEnergyUse</t>
   </si>
   <si>
-    <t>ActivityProfWD</t>
-  </si>
-  <si>
-    <t>ActivityProfWE</t>
-  </si>
-  <si>
     <t>Timezone</t>
   </si>
   <si>
@@ -738,6 +732,15 @@
   </si>
   <si>
     <t>Kotthaus and Grimmond (2013, 2014a, 2014b)</t>
+  </si>
+  <si>
+    <t>QF0_BEU_WD</t>
+  </si>
+  <si>
+    <t>QF0_BEU_WE</t>
+  </si>
+  <si>
+    <t>old</t>
   </si>
 </sst>
 </file>
@@ -1234,12 +1237,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1582,1031 +1586,1309 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DB73"/>
+  <dimension ref="A1:CZ67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="22.42578125" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="41" max="41" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="15" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="12" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="15" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="20" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="19" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="22" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="19" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="12" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="19" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="12" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="19" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="12" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="19" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="12" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="19" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="12" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="19" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="12" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="19" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="12" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="19" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="12" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="21" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="21" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="86" max="88" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="89" max="91" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="92" max="96" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="97" max="101" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="1.7109375" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="41.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:106" x14ac:dyDescent="0.25">
-      <c r="A1">
+    <row r="1" spans="1:104" x14ac:dyDescent="0.25">
+      <c r="A1" s="5">
         <v>1</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="5">
         <v>2</v>
       </c>
-      <c r="C1">
+      <c r="C1" s="5">
         <v>3</v>
       </c>
-      <c r="D1">
+      <c r="D1" s="5">
         <v>4</v>
       </c>
-      <c r="E1">
+      <c r="E1" s="5">
         <v>5</v>
       </c>
-      <c r="F1">
+      <c r="F1" s="5">
         <v>6</v>
       </c>
-      <c r="G1">
+      <c r="G1" s="5">
         <v>7</v>
       </c>
-      <c r="H1">
+      <c r="H1" s="5">
         <v>8</v>
       </c>
-      <c r="I1">
+      <c r="I1" s="5">
         <v>9</v>
       </c>
-      <c r="J1">
+      <c r="J1" s="5">
         <v>10</v>
       </c>
-      <c r="K1">
+      <c r="K1" s="5">
         <v>11</v>
       </c>
-      <c r="L1">
+      <c r="L1" s="5">
         <v>12</v>
       </c>
-      <c r="M1">
+      <c r="M1" s="5">
         <v>13</v>
       </c>
-      <c r="N1">
+      <c r="N1" s="5">
         <v>14</v>
       </c>
-      <c r="O1">
+      <c r="O1" s="5">
         <v>15</v>
       </c>
-      <c r="P1">
+      <c r="P1" s="5">
         <v>16</v>
       </c>
-      <c r="Q1">
+      <c r="Q1" s="5">
         <v>17</v>
       </c>
-      <c r="R1">
+      <c r="R1" s="5">
         <v>18</v>
       </c>
-      <c r="S1">
+      <c r="S1" s="5">
         <v>19</v>
       </c>
-      <c r="T1">
+      <c r="T1" s="5">
         <v>20</v>
       </c>
-      <c r="U1">
+      <c r="U1" s="5">
         <v>21</v>
       </c>
-      <c r="V1">
+      <c r="V1" s="5">
         <v>22</v>
       </c>
-      <c r="W1">
+      <c r="W1" s="5">
         <v>23</v>
       </c>
-      <c r="X1">
+      <c r="X1" s="5">
         <v>24</v>
       </c>
-      <c r="Y1">
+      <c r="Y1" s="5">
         <v>25</v>
       </c>
-      <c r="Z1">
+      <c r="Z1" s="5">
         <v>26</v>
       </c>
-      <c r="AA1">
+      <c r="AA1" s="5">
         <v>27</v>
       </c>
-      <c r="AB1">
+      <c r="AB1" s="5">
         <v>28</v>
       </c>
-      <c r="AC1">
+      <c r="AC1" s="5">
         <v>29</v>
       </c>
-      <c r="AD1">
+      <c r="AD1" s="5">
         <v>30</v>
       </c>
-      <c r="AE1">
+      <c r="AE1" s="5">
         <v>31</v>
       </c>
-      <c r="AF1">
+      <c r="AF1" s="5">
         <v>32</v>
       </c>
-      <c r="AG1">
+      <c r="AG1" s="5">
         <v>33</v>
       </c>
-      <c r="AH1">
+      <c r="AH1" s="5">
         <v>34</v>
       </c>
-      <c r="AI1">
+      <c r="AI1" s="5">
         <v>35</v>
       </c>
-      <c r="AJ1">
+      <c r="AJ1" s="5">
         <v>36</v>
       </c>
-      <c r="AK1">
+      <c r="AK1" s="5">
         <v>37</v>
       </c>
-      <c r="AL1">
+      <c r="AL1" s="5">
         <v>38</v>
       </c>
-      <c r="AM1">
+      <c r="AM1" s="5">
         <v>39</v>
       </c>
-      <c r="AN1">
+      <c r="AN1" s="5">
         <v>40</v>
       </c>
-      <c r="AO1">
+      <c r="AO1" s="5">
         <v>41</v>
       </c>
-      <c r="AP1">
+      <c r="AP1" s="5">
         <v>42</v>
       </c>
-      <c r="AQ1">
+      <c r="AQ1" s="5">
         <v>43</v>
       </c>
-      <c r="AR1">
+      <c r="AR1" s="5">
         <v>44</v>
       </c>
-      <c r="AS1">
+      <c r="AS1" s="5">
         <v>45</v>
       </c>
-      <c r="AT1">
+      <c r="AT1" s="5">
         <v>46</v>
       </c>
-      <c r="AU1">
+      <c r="AU1" s="5">
         <v>47</v>
       </c>
-      <c r="AV1">
+      <c r="AV1" s="5">
         <v>48</v>
       </c>
-      <c r="AW1">
+      <c r="AW1" s="5">
         <v>49</v>
       </c>
-      <c r="AX1">
+      <c r="AX1" s="5">
         <v>50</v>
       </c>
-      <c r="AY1">
+      <c r="AY1" s="5">
         <v>51</v>
       </c>
-      <c r="AZ1">
+      <c r="AZ1" s="5">
         <v>52</v>
       </c>
-      <c r="BA1">
+      <c r="BA1" s="5">
         <v>53</v>
       </c>
-      <c r="BB1">
+      <c r="BB1" s="5">
         <v>54</v>
       </c>
-      <c r="BC1">
+      <c r="BC1" s="5">
         <v>55</v>
       </c>
-      <c r="BD1">
+      <c r="BD1" s="5">
         <v>56</v>
       </c>
-      <c r="BE1">
+      <c r="BE1" s="5">
         <v>57</v>
       </c>
-      <c r="BF1">
+      <c r="BF1" s="5">
         <v>58</v>
       </c>
-      <c r="BG1">
+      <c r="BG1" s="5">
         <v>59</v>
       </c>
-      <c r="BH1">
+      <c r="BH1" s="5">
         <v>60</v>
       </c>
-      <c r="BI1">
+      <c r="BI1" s="5">
         <v>61</v>
       </c>
-      <c r="BJ1">
+      <c r="BJ1" s="5">
         <v>62</v>
       </c>
-      <c r="BK1">
+      <c r="BK1" s="5">
         <v>63</v>
       </c>
-      <c r="BL1">
+      <c r="BL1" s="5">
         <v>64</v>
       </c>
-      <c r="BM1">
+      <c r="BM1" s="5">
         <v>65</v>
       </c>
-      <c r="BN1">
+      <c r="BN1" s="5">
         <v>66</v>
       </c>
-      <c r="BO1">
+      <c r="BO1" s="5">
         <v>67</v>
       </c>
-      <c r="BP1">
+      <c r="BP1" s="5">
         <v>68</v>
       </c>
-      <c r="BQ1">
+      <c r="BQ1" s="5">
         <v>69</v>
       </c>
-      <c r="BR1">
+      <c r="BR1" s="5">
         <v>70</v>
       </c>
-      <c r="BS1">
+      <c r="BS1" s="5">
         <v>71</v>
       </c>
-      <c r="BT1">
+      <c r="BT1" s="5">
         <v>72</v>
       </c>
-      <c r="BU1">
+      <c r="BU1" s="5">
         <v>73</v>
       </c>
-      <c r="BV1">
+      <c r="BV1" s="5">
         <v>74</v>
       </c>
-      <c r="BW1">
+      <c r="BW1" s="5">
         <v>75</v>
       </c>
-      <c r="BX1">
+      <c r="BX1" s="5">
         <v>76</v>
       </c>
-      <c r="BY1">
+      <c r="BY1" s="5">
         <v>77</v>
       </c>
-      <c r="BZ1">
+      <c r="BZ1" s="5">
         <v>78</v>
       </c>
-      <c r="CA1">
+      <c r="CA1" s="5">
         <v>79</v>
       </c>
-      <c r="CB1">
-        <v>80</v>
-      </c>
-      <c r="CC1">
+      <c r="CB1" s="5">
+        <v>80</v>
+      </c>
+      <c r="CC1" s="5">
         <v>81</v>
       </c>
-      <c r="CD1">
+      <c r="CD1" s="5">
         <v>82</v>
       </c>
-      <c r="CE1">
+      <c r="CE1" s="5">
         <v>83</v>
       </c>
-      <c r="CF1">
+      <c r="CF1" s="5">
         <v>84</v>
       </c>
-      <c r="CG1">
+      <c r="CG1" s="5">
         <v>85</v>
       </c>
-      <c r="CH1">
+      <c r="CH1" s="5">
         <v>86</v>
       </c>
-      <c r="CI1">
+      <c r="CI1" s="5">
         <v>87</v>
       </c>
-      <c r="CJ1">
+      <c r="CJ1" s="5">
         <v>88</v>
       </c>
-      <c r="CK1">
+      <c r="CK1" s="5">
         <v>89</v>
       </c>
-      <c r="CL1">
+      <c r="CL1" s="5">
         <v>90</v>
       </c>
-      <c r="CM1">
+      <c r="CM1" s="5">
         <v>91</v>
       </c>
-      <c r="CN1">
+      <c r="CN1" s="5">
         <v>92</v>
       </c>
-      <c r="CO1">
+      <c r="CO1" s="5">
         <v>93</v>
       </c>
-      <c r="CP1">
+      <c r="CP1" s="5">
         <v>94</v>
       </c>
-      <c r="CQ1">
+      <c r="CQ1" s="5">
         <v>95</v>
       </c>
-      <c r="CR1">
+      <c r="CR1" s="5">
         <v>96</v>
       </c>
-      <c r="CS1">
+      <c r="CS1" s="5">
         <v>97</v>
       </c>
-      <c r="CT1">
+      <c r="CT1" s="5">
         <v>98</v>
       </c>
-      <c r="CU1">
+      <c r="CU1" s="5">
         <v>99</v>
       </c>
-      <c r="CV1">
+      <c r="CV1" s="5">
         <v>100</v>
       </c>
-      <c r="CW1">
+      <c r="CW1" s="5">
         <v>101</v>
       </c>
-      <c r="CX1">
-        <v>102</v>
-      </c>
-      <c r="CY1">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="2" spans="1:106" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="CX1" s="5"/>
+      <c r="CY1" s="5"/>
+      <c r="CZ1" s="5"/>
+    </row>
+    <row r="2" spans="1:104" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="V2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="W2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="X2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AG2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="AH2" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="AI2" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="AJ2" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="AK2" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="AL2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AM2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="AN2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AO2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="AP2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AQ2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AR2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="AS2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="AT2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="AU2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="AV2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="AW2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="AX2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="AY2" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="AZ2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="BA2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="BB2" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="BC2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="BD2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="BE2" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="BF2" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="BG2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="BH2" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="BI2" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="BJ2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="BK2" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="BL2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="BM2" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="BN2" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="BO2" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="BP2" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="BQ2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="BR2" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="BS2" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="BT2" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="BU2" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="BV2" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="BW2" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="BX2" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BY2" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="BZ2" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="CA2" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="CB2" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="CC2" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="CD2" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="CE2" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="CF2" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="CG2" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="CH2" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="CI2" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="CJ2" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="CK2" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="CL2" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="CM2" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="CN2" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="CO2" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="CP2" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="CQ2" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="CR2" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="CS2" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="CT2" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="CU2" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="CV2" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="CW2" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="CX2" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="CY2" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="CZ2" s="5" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="3" spans="1:104" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>98</v>
+      </c>
+      <c r="B3" s="5">
+        <v>2012</v>
+      </c>
+      <c r="C3" s="5">
+        <v>85</v>
+      </c>
+      <c r="D3" s="5">
+        <v>302</v>
+      </c>
+      <c r="E3" s="5">
+        <v>51.51</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0.12</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0</v>
+      </c>
+      <c r="H3" s="5">
+        <v>2221.56</v>
+      </c>
+      <c r="I3" s="5">
+        <v>10.7</v>
+      </c>
+      <c r="J3" s="5">
+        <v>49.6</v>
+      </c>
+      <c r="K3" s="5">
+        <v>1</v>
+      </c>
+      <c r="L3" s="5">
+        <v>0</v>
+      </c>
+      <c r="M3" s="5">
+        <v>0</v>
+      </c>
+      <c r="N3" s="5">
+        <v>0.43</v>
+      </c>
+      <c r="O3" s="5">
+        <v>0.38</v>
+      </c>
+      <c r="P3" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="R3" s="5">
+        <v>0.03</v>
+      </c>
+      <c r="S3" s="5">
+        <v>0</v>
+      </c>
+      <c r="T3" s="5">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="U3" s="5">
+        <v>0</v>
+      </c>
+      <c r="V3" s="5">
+        <v>0</v>
+      </c>
+      <c r="W3" s="5">
+        <v>0</v>
+      </c>
+      <c r="X3" s="5">
+        <v>22</v>
+      </c>
+      <c r="Y3" s="5">
+        <v>13.1</v>
+      </c>
+      <c r="Z3" s="5">
+        <v>13.1</v>
+      </c>
+      <c r="AA3" s="5">
+        <v>1.9</v>
+      </c>
+      <c r="AB3" s="5">
+        <v>14.2</v>
+      </c>
+      <c r="AC3" s="5">
+        <v>-999</v>
+      </c>
+      <c r="AD3" s="5">
+        <v>-999</v>
+      </c>
+      <c r="AE3" s="5">
+        <v>-999</v>
+      </c>
+      <c r="AF3" s="5">
+        <v>-999</v>
+      </c>
+      <c r="AG3" s="5">
+        <v>204.58</v>
+      </c>
+      <c r="AH3" s="5">
+        <v>-999</v>
+      </c>
+      <c r="AI3" s="5">
+        <v>-999</v>
+      </c>
+      <c r="AJ3" s="5">
+        <v>0.88</v>
+      </c>
+      <c r="AK3" s="5">
+        <v>0.88</v>
+      </c>
+      <c r="AL3" s="5">
+        <v>661</v>
+      </c>
+      <c r="AM3" s="5">
+        <v>662</v>
+      </c>
+      <c r="AN3" s="5">
+        <v>661</v>
+      </c>
+      <c r="AO3" s="5">
+        <v>662</v>
+      </c>
+      <c r="AP3" s="5">
+        <v>663</v>
+      </c>
+      <c r="AQ3" s="5">
+        <v>663</v>
+      </c>
+      <c r="AR3" s="5">
+        <v>661</v>
+      </c>
+      <c r="AS3" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="AT3" s="5">
+        <v>1</v>
+      </c>
+      <c r="AU3" s="5">
+        <v>10</v>
+      </c>
+      <c r="AV3" s="5">
+        <v>1</v>
+      </c>
+      <c r="AW3" s="5">
+        <v>200</v>
+      </c>
+      <c r="AX3" s="5">
+        <v>99999</v>
+      </c>
+      <c r="AY3" s="5">
+        <v>99999</v>
+      </c>
+      <c r="AZ3" s="5">
+        <v>99999</v>
+      </c>
+      <c r="BA3" s="5">
+        <v>661</v>
+      </c>
+      <c r="BB3" s="5">
+        <v>99999</v>
+      </c>
+      <c r="BC3" s="5">
+        <v>99999</v>
+      </c>
+      <c r="BD3" s="5">
+        <v>99999</v>
+      </c>
+      <c r="BE3" s="5">
+        <v>99999</v>
+      </c>
+      <c r="BF3" s="5">
+        <v>99999</v>
+      </c>
+      <c r="BG3" s="5">
+        <v>0</v>
+      </c>
+      <c r="BH3" s="5">
+        <v>0</v>
+      </c>
+      <c r="BI3" s="5">
+        <v>100</v>
+      </c>
+      <c r="BJ3" s="5">
+        <v>0</v>
+      </c>
+      <c r="BK3" s="5">
+        <v>0</v>
+      </c>
+      <c r="BL3" s="5">
+        <v>0</v>
+      </c>
+      <c r="BM3" s="5">
+        <v>0</v>
+      </c>
+      <c r="BN3" s="5">
+        <v>0</v>
+      </c>
+      <c r="BO3" s="5">
+        <v>0</v>
+      </c>
+      <c r="BP3" s="5">
+        <v>0</v>
+      </c>
+      <c r="BQ3" s="5">
+        <v>0</v>
+      </c>
+      <c r="BR3" s="5">
+        <v>0</v>
+      </c>
+      <c r="BS3" s="5">
+        <v>0</v>
+      </c>
+      <c r="BT3" s="5">
+        <v>0</v>
+      </c>
+      <c r="BU3" s="5">
+        <v>0</v>
+      </c>
+      <c r="BV3" s="5">
+        <v>0</v>
+      </c>
+      <c r="BW3" s="5">
+        <v>0</v>
+      </c>
+      <c r="BX3" s="5">
+        <v>0</v>
+      </c>
+      <c r="BY3" s="5">
+        <v>0</v>
+      </c>
+      <c r="BZ3" s="5">
+        <v>661</v>
+      </c>
+      <c r="CA3" s="5">
+        <v>662</v>
+      </c>
+      <c r="CB3" s="5">
+        <v>663</v>
+      </c>
+      <c r="CC3" s="5">
+        <v>664</v>
+      </c>
+      <c r="CD3" s="5">
+        <v>665</v>
+      </c>
+      <c r="CE3" s="5">
+        <v>666</v>
+      </c>
+      <c r="CF3" s="5">
+        <v>667</v>
+      </c>
+      <c r="CG3" s="5">
+        <v>1.08</v>
+      </c>
+      <c r="CH3" s="5">
+        <v>0.15</v>
+      </c>
+      <c r="CI3" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="CJ3" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="CK3" s="5">
+        <v>806</v>
+      </c>
+      <c r="CL3" s="5">
+        <v>807</v>
+      </c>
+      <c r="CM3" s="5">
+        <v>808</v>
+      </c>
+      <c r="CN3" s="5">
+        <v>0.15</v>
+      </c>
+      <c r="CO3" s="5">
+        <v>0.45</v>
+      </c>
+      <c r="CP3" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="CQ3" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="CR3" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="CS3" s="5">
+        <v>801</v>
+      </c>
+      <c r="CT3" s="5">
+        <v>8021</v>
+      </c>
+      <c r="CU3" s="5">
+        <v>8022</v>
+      </c>
+      <c r="CV3" s="5">
+        <v>803</v>
+      </c>
+      <c r="CW3" s="5">
+        <v>8041</v>
+      </c>
+      <c r="CX3" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="CY3" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="CZ3" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="H2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" t="s">
-        <v>238</v>
-      </c>
-      <c r="K2" t="s">
-        <v>8</v>
-      </c>
-      <c r="L2" t="s">
-        <v>9</v>
-      </c>
-      <c r="M2" t="s">
-        <v>10</v>
-      </c>
-      <c r="N2" t="s">
-        <v>11</v>
-      </c>
-      <c r="O2" t="s">
-        <v>12</v>
-      </c>
-      <c r="P2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>14</v>
-      </c>
-      <c r="R2" t="s">
-        <v>15</v>
-      </c>
-      <c r="S2" t="s">
-        <v>16</v>
-      </c>
-      <c r="T2" t="s">
-        <v>17</v>
-      </c>
-      <c r="U2" t="s">
-        <v>18</v>
-      </c>
-      <c r="V2" t="s">
-        <v>19</v>
-      </c>
-      <c r="W2" t="s">
-        <v>20</v>
-      </c>
-      <c r="X2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>24</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>25</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>28</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>233</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>234</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>31</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>33</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>34</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>35</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>38</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>39</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>40</v>
-      </c>
-      <c r="AT2" t="s">
-        <v>41</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>43</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>47</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>48</v>
-      </c>
-      <c r="BB2" t="s">
-        <v>235</v>
-      </c>
-      <c r="BC2" t="s">
-        <v>236</v>
-      </c>
-      <c r="BD2" t="s">
-        <v>49</v>
-      </c>
-      <c r="BE2" t="s">
-        <v>50</v>
-      </c>
-      <c r="BF2" t="s">
-        <v>51</v>
-      </c>
-      <c r="BG2" t="s">
-        <v>52</v>
-      </c>
-      <c r="BH2" t="s">
-        <v>53</v>
-      </c>
-      <c r="BI2" t="s">
-        <v>54</v>
-      </c>
-      <c r="BJ2" t="s">
-        <v>55</v>
-      </c>
-      <c r="BK2" t="s">
-        <v>56</v>
-      </c>
-      <c r="BL2" t="s">
-        <v>57</v>
-      </c>
-      <c r="BM2" t="s">
-        <v>58</v>
-      </c>
-      <c r="BN2" t="s">
-        <v>59</v>
-      </c>
-      <c r="BO2" t="s">
-        <v>60</v>
-      </c>
-      <c r="BP2" t="s">
-        <v>61</v>
-      </c>
-      <c r="BQ2" t="s">
-        <v>62</v>
-      </c>
-      <c r="BR2" t="s">
-        <v>63</v>
-      </c>
-      <c r="BS2" t="s">
-        <v>64</v>
-      </c>
-      <c r="BT2" t="s">
-        <v>65</v>
-      </c>
-      <c r="BU2" t="s">
-        <v>66</v>
-      </c>
-      <c r="BV2" t="s">
-        <v>67</v>
-      </c>
-      <c r="BW2" t="s">
-        <v>68</v>
-      </c>
-      <c r="BX2" t="s">
-        <v>69</v>
-      </c>
-      <c r="BY2" t="s">
-        <v>70</v>
-      </c>
-      <c r="BZ2" t="s">
-        <v>71</v>
-      </c>
-      <c r="CA2" t="s">
-        <v>72</v>
-      </c>
-      <c r="CB2" t="s">
-        <v>73</v>
-      </c>
-      <c r="CC2" t="s">
-        <v>74</v>
-      </c>
-      <c r="CD2" t="s">
-        <v>75</v>
-      </c>
-      <c r="CE2" t="s">
-        <v>76</v>
-      </c>
-      <c r="CF2" t="s">
-        <v>77</v>
-      </c>
-      <c r="CG2" t="s">
-        <v>78</v>
-      </c>
-      <c r="CH2" t="s">
-        <v>79</v>
-      </c>
-      <c r="CI2" t="s">
-        <v>214</v>
-      </c>
-      <c r="CJ2" t="s">
-        <v>215</v>
-      </c>
-      <c r="CK2" t="s">
-        <v>216</v>
-      </c>
-      <c r="CL2" t="s">
-        <v>217</v>
-      </c>
-      <c r="CM2" t="s">
-        <v>218</v>
-      </c>
-      <c r="CN2" t="s">
-        <v>219</v>
-      </c>
-      <c r="CO2" t="s">
-        <v>220</v>
-      </c>
-      <c r="CP2" t="s">
-        <v>221</v>
-      </c>
-      <c r="CQ2" t="s">
-        <v>222</v>
-      </c>
-      <c r="CR2" t="s">
-        <v>223</v>
-      </c>
-      <c r="CS2" t="s">
-        <v>224</v>
-      </c>
-      <c r="CT2" t="s">
-        <v>225</v>
-      </c>
-      <c r="CU2" t="s">
-        <v>226</v>
-      </c>
-      <c r="CV2" t="s">
-        <v>227</v>
-      </c>
-      <c r="CW2" t="s">
-        <v>228</v>
-      </c>
-      <c r="CX2" t="s">
-        <v>229</v>
-      </c>
-      <c r="CY2" t="s">
-        <v>230</v>
-      </c>
-      <c r="CZ2" t="s">
-        <v>80</v>
-      </c>
-      <c r="DA2" t="s">
-        <v>231</v>
-      </c>
-      <c r="DB2" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="3" spans="1:106" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>2012</v>
-      </c>
-      <c r="C3">
-        <v>85</v>
-      </c>
-      <c r="D3">
-        <v>302</v>
-      </c>
-      <c r="E3">
-        <v>51.51</v>
-      </c>
-      <c r="F3">
-        <v>0.12</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>2221.56</v>
-      </c>
-      <c r="I3">
-        <v>10.7</v>
-      </c>
-      <c r="J3">
-        <v>49.6</v>
-      </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>0.43</v>
-      </c>
-      <c r="O3">
-        <v>0.38</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <v>0.02</v>
-      </c>
-      <c r="R3">
-        <v>0.03</v>
-      </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
-      <c r="T3">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="U3">
-        <v>0</v>
-      </c>
-      <c r="V3">
-        <v>0</v>
-      </c>
-      <c r="W3">
-        <v>0</v>
-      </c>
-      <c r="X3">
-        <v>22</v>
-      </c>
-      <c r="Y3">
-        <v>13.1</v>
-      </c>
-      <c r="Z3">
-        <v>13.1</v>
-      </c>
-      <c r="AA3">
-        <v>1.9</v>
-      </c>
-      <c r="AB3">
-        <v>14.2</v>
-      </c>
-      <c r="AC3">
-        <v>-999</v>
-      </c>
-      <c r="AD3">
-        <v>-999</v>
-      </c>
-      <c r="AE3">
-        <v>-999</v>
-      </c>
-      <c r="AF3">
-        <v>-999</v>
-      </c>
-      <c r="AG3">
-        <v>204.58</v>
-      </c>
-      <c r="AH3">
-        <v>-999</v>
-      </c>
-      <c r="AI3">
-        <v>-999</v>
-      </c>
-      <c r="AJ3">
-        <v>661</v>
-      </c>
-      <c r="AK3">
-        <v>662</v>
-      </c>
-      <c r="AL3">
-        <v>661</v>
-      </c>
-      <c r="AM3">
-        <v>662</v>
-      </c>
-      <c r="AN3">
-        <v>663</v>
-      </c>
-      <c r="AO3">
-        <v>663</v>
-      </c>
-      <c r="AP3">
-        <v>661</v>
-      </c>
-      <c r="AQ3">
-        <v>0.25</v>
-      </c>
-      <c r="AR3">
-        <v>1</v>
-      </c>
-      <c r="AS3">
-        <v>10</v>
-      </c>
-      <c r="AT3">
-        <v>1</v>
-      </c>
-      <c r="AU3">
-        <v>200</v>
-      </c>
-      <c r="AV3">
-        <v>99999</v>
-      </c>
-      <c r="AW3">
-        <v>99999</v>
-      </c>
-      <c r="AX3">
-        <v>99999</v>
-      </c>
-      <c r="AY3">
-        <v>661</v>
-      </c>
-      <c r="AZ3">
-        <v>661</v>
-      </c>
-      <c r="BA3">
-        <v>662</v>
-      </c>
-      <c r="BB3">
-        <v>90000</v>
-      </c>
-      <c r="BC3">
-        <v>90000</v>
-      </c>
-      <c r="BD3">
-        <v>99999</v>
-      </c>
-      <c r="BE3">
-        <v>99999</v>
-      </c>
-      <c r="BF3">
-        <v>99999</v>
-      </c>
-      <c r="BG3">
-        <v>99999</v>
-      </c>
-      <c r="BH3">
-        <v>99999</v>
-      </c>
-      <c r="BI3">
-        <v>0</v>
-      </c>
-      <c r="BJ3">
-        <v>0</v>
-      </c>
-      <c r="BK3">
-        <v>100</v>
-      </c>
-      <c r="BL3">
-        <v>0</v>
-      </c>
-      <c r="BM3">
-        <v>0</v>
-      </c>
-      <c r="BN3">
-        <v>0</v>
-      </c>
-      <c r="BO3">
-        <v>0</v>
-      </c>
-      <c r="BP3">
-        <v>0</v>
-      </c>
-      <c r="BQ3">
-        <v>0</v>
-      </c>
-      <c r="BR3">
-        <v>0</v>
-      </c>
-      <c r="BS3">
-        <v>0</v>
-      </c>
-      <c r="BT3">
-        <v>0</v>
-      </c>
-      <c r="BU3">
-        <v>0</v>
-      </c>
-      <c r="BV3">
-        <v>0</v>
-      </c>
-      <c r="BW3">
-        <v>0</v>
-      </c>
-      <c r="BX3">
-        <v>0</v>
-      </c>
-      <c r="BY3">
-        <v>0</v>
-      </c>
-      <c r="BZ3">
-        <v>0</v>
-      </c>
-      <c r="CA3">
-        <v>0</v>
-      </c>
-      <c r="CB3">
-        <v>661</v>
-      </c>
-      <c r="CC3">
-        <v>662</v>
-      </c>
-      <c r="CD3">
-        <v>663</v>
-      </c>
-      <c r="CE3">
-        <v>664</v>
-      </c>
-      <c r="CF3">
-        <v>665</v>
-      </c>
-      <c r="CG3">
-        <v>666</v>
-      </c>
-      <c r="CH3">
-        <v>667</v>
-      </c>
-      <c r="CI3">
-        <v>1.08</v>
-      </c>
-      <c r="CJ3">
-        <v>0.15</v>
-      </c>
-      <c r="CK3">
-        <v>0.05</v>
-      </c>
-      <c r="CL3">
-        <v>0.8</v>
-      </c>
-      <c r="CM3">
-        <v>806</v>
-      </c>
-      <c r="CN3">
-        <v>807</v>
-      </c>
-      <c r="CO3">
-        <v>808</v>
-      </c>
-      <c r="CP3">
-        <v>0.15</v>
-      </c>
-      <c r="CQ3">
-        <v>0.45</v>
-      </c>
-      <c r="CR3">
-        <v>0.05</v>
-      </c>
-      <c r="CS3">
-        <v>0.1</v>
-      </c>
-      <c r="CT3">
-        <v>0.25</v>
-      </c>
-      <c r="CU3">
-        <v>801</v>
-      </c>
-      <c r="CV3">
-        <v>802</v>
-      </c>
-      <c r="CW3">
-        <v>803</v>
-      </c>
-      <c r="CX3">
-        <v>804</v>
-      </c>
-      <c r="CY3">
-        <v>805</v>
-      </c>
-      <c r="CZ3" t="s">
-        <v>80</v>
-      </c>
-      <c r="DA3" t="s">
-        <v>81</v>
-      </c>
-      <c r="DB3" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="4" spans="1:106" x14ac:dyDescent="0.25">
-      <c r="A4">
+    </row>
+    <row r="4" spans="1:104" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
         <v>-9</v>
       </c>
-    </row>
-    <row r="5" spans="1:106" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
+      <c r="V4" s="5"/>
+      <c r="W4" s="5"/>
+      <c r="X4" s="5"/>
+      <c r="Y4" s="5"/>
+      <c r="Z4" s="5"/>
+      <c r="AA4" s="5"/>
+      <c r="AB4" s="5"/>
+      <c r="AC4" s="5"/>
+      <c r="AD4" s="5"/>
+      <c r="AE4" s="5"/>
+      <c r="AF4" s="5"/>
+      <c r="AG4" s="5"/>
+      <c r="AH4" s="5"/>
+      <c r="AI4" s="5"/>
+      <c r="AJ4" s="5"/>
+      <c r="AK4" s="5"/>
+      <c r="AL4" s="5"/>
+      <c r="AM4" s="5"/>
+      <c r="AN4" s="5"/>
+      <c r="AO4" s="5"/>
+      <c r="AP4" s="5"/>
+      <c r="AQ4" s="5"/>
+      <c r="AR4" s="5"/>
+      <c r="AS4" s="5"/>
+      <c r="AT4" s="5"/>
+      <c r="AU4" s="5"/>
+      <c r="AV4" s="5"/>
+      <c r="AW4" s="5"/>
+      <c r="AX4" s="5"/>
+      <c r="AY4" s="5"/>
+      <c r="AZ4" s="5"/>
+      <c r="BA4" s="5"/>
+      <c r="BB4" s="5"/>
+      <c r="BC4" s="5"/>
+      <c r="BD4" s="5"/>
+      <c r="BE4" s="5"/>
+      <c r="BF4" s="5"/>
+      <c r="BG4" s="5"/>
+      <c r="BH4" s="5"/>
+      <c r="BI4" s="5"/>
+      <c r="BJ4" s="5"/>
+      <c r="BK4" s="5"/>
+      <c r="BL4" s="5"/>
+      <c r="BM4" s="5"/>
+      <c r="BN4" s="5"/>
+      <c r="BO4" s="5"/>
+      <c r="BP4" s="5"/>
+      <c r="BQ4" s="5"/>
+      <c r="BR4" s="5"/>
+      <c r="BS4" s="5"/>
+      <c r="BT4" s="5"/>
+      <c r="BU4" s="5"/>
+      <c r="BV4" s="5"/>
+      <c r="BW4" s="5"/>
+      <c r="BX4" s="5"/>
+      <c r="BY4" s="5"/>
+      <c r="BZ4" s="5"/>
+      <c r="CA4" s="5"/>
+      <c r="CB4" s="5"/>
+      <c r="CC4" s="5"/>
+      <c r="CD4" s="5"/>
+      <c r="CE4" s="5"/>
+      <c r="CF4" s="5"/>
+      <c r="CG4" s="5"/>
+      <c r="CH4" s="5"/>
+      <c r="CI4" s="5"/>
+      <c r="CJ4" s="5"/>
+      <c r="CK4" s="5"/>
+      <c r="CL4" s="5"/>
+      <c r="CM4" s="5"/>
+      <c r="CN4" s="5"/>
+      <c r="CO4" s="5"/>
+      <c r="CP4" s="5"/>
+      <c r="CQ4" s="5"/>
+      <c r="CR4" s="5"/>
+      <c r="CS4" s="5"/>
+      <c r="CT4" s="5"/>
+      <c r="CU4" s="5"/>
+      <c r="CV4" s="5"/>
+      <c r="CW4" s="5"/>
+      <c r="CX4" s="5"/>
+      <c r="CY4" s="5"/>
+      <c r="CZ4" s="5"/>
+    </row>
+    <row r="5" spans="1:104" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
         <v>-9</v>
       </c>
-    </row>
-    <row r="6" spans="1:106" x14ac:dyDescent="0.25">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5"/>
+      <c r="W5" s="5"/>
+      <c r="X5" s="5"/>
+      <c r="Y5" s="5"/>
+      <c r="Z5" s="5"/>
+      <c r="AA5" s="5"/>
+      <c r="AB5" s="5"/>
+      <c r="AC5" s="5"/>
+      <c r="AD5" s="5"/>
+      <c r="AE5" s="5"/>
+      <c r="AF5" s="5"/>
+      <c r="AG5" s="5"/>
+      <c r="AH5" s="5"/>
+      <c r="AI5" s="5"/>
+      <c r="AJ5" s="5"/>
+      <c r="AK5" s="5"/>
+      <c r="AL5" s="5"/>
+      <c r="AM5" s="5"/>
+      <c r="AN5" s="5"/>
+      <c r="AO5" s="5"/>
+      <c r="AP5" s="5"/>
+      <c r="AQ5" s="5"/>
+      <c r="AR5" s="5"/>
+      <c r="AS5" s="5"/>
+      <c r="AT5" s="5"/>
+      <c r="AU5" s="5"/>
+      <c r="AV5" s="5"/>
+      <c r="AW5" s="5"/>
+      <c r="AX5" s="5"/>
+      <c r="AY5" s="5"/>
+      <c r="AZ5" s="5"/>
+      <c r="BA5" s="5"/>
+      <c r="BB5" s="5"/>
+      <c r="BC5" s="5"/>
+      <c r="BD5" s="5"/>
+      <c r="BE5" s="5"/>
+      <c r="BF5" s="5"/>
+      <c r="BG5" s="5"/>
+      <c r="BH5" s="5"/>
+      <c r="BI5" s="5"/>
+      <c r="BJ5" s="5"/>
+      <c r="BK5" s="5"/>
+      <c r="BL5" s="5"/>
+      <c r="BM5" s="5"/>
+      <c r="BN5" s="5"/>
+      <c r="BO5" s="5"/>
+      <c r="BP5" s="5"/>
+      <c r="BQ5" s="5"/>
+      <c r="BR5" s="5"/>
+      <c r="BS5" s="5"/>
+      <c r="BT5" s="5"/>
+      <c r="BU5" s="5"/>
+      <c r="BV5" s="5"/>
+      <c r="BW5" s="5"/>
+      <c r="BX5" s="5"/>
+      <c r="BY5" s="5"/>
+      <c r="BZ5" s="5"/>
+      <c r="CA5" s="5"/>
+      <c r="CB5" s="5"/>
+      <c r="CC5" s="5"/>
+      <c r="CD5" s="5"/>
+      <c r="CE5" s="5"/>
+      <c r="CF5" s="5"/>
+      <c r="CG5" s="5"/>
+      <c r="CH5" s="5"/>
+      <c r="CI5" s="5"/>
+      <c r="CJ5" s="5"/>
+      <c r="CK5" s="5"/>
+      <c r="CL5" s="5"/>
+      <c r="CM5" s="5"/>
+      <c r="CN5" s="5"/>
+      <c r="CO5" s="5"/>
+      <c r="CP5" s="5"/>
+      <c r="CQ5" s="5"/>
+      <c r="CR5" s="5"/>
+      <c r="CS5" s="5"/>
+      <c r="CT5" s="5"/>
+      <c r="CU5" s="5"/>
+      <c r="CV5" s="5"/>
+      <c r="CW5" s="5"/>
+      <c r="CX5" s="5"/>
+      <c r="CY5" s="5"/>
+      <c r="CZ5" s="5"/>
+    </row>
+    <row r="6" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:106" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:106" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:106" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:106" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:106" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:106" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:106" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:106" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:106" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:106" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>80</v>
       </c>
@@ -2866,48 +3148,18 @@
         <v>80</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>80</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I82"/>
+  <dimension ref="A1:I106"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="F91" sqref="F91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="54" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3100,52 +3352,41 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" t="s">
-        <v>91</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="G8" t="s">
-        <v>185</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="I8" t="s">
-        <v>211</v>
-      </c>
+      <c r="B8" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="5"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>92</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>93</v>
-      </c>
-      <c r="E9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>167</v>
-      </c>
-      <c r="F9" t="s">
-        <v>208</v>
       </c>
       <c r="G9" t="s">
         <v>185</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>182</v>
+      </c>
+      <c r="I9" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -3153,61 +3394,60 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D10" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="E10" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F10" t="s">
-        <v>183</v>
+        <v>208</v>
       </c>
       <c r="G10" t="s">
-        <v>186</v>
-      </c>
-      <c r="H10" s="3"/>
+        <v>185</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" t="s">
-        <v>95</v>
-      </c>
-      <c r="E11" t="s">
-        <v>170</v>
-      </c>
-      <c r="F11" t="s">
-        <v>184</v>
-      </c>
-      <c r="G11" t="s">
-        <v>186</v>
-      </c>
+      <c r="B11" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
       <c r="H11" s="3"/>
+      <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>96</v>
+        <v>94</v>
+      </c>
+      <c r="D12" t="s">
+        <v>86</v>
       </c>
       <c r="E12" t="s">
         <v>170</v>
       </c>
       <c r="F12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G12" t="s">
         <v>186</v>
@@ -3219,47 +3459,49 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>97</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>171</v>
+        <v>95</v>
+      </c>
+      <c r="E13" t="s">
+        <v>170</v>
+      </c>
+      <c r="F13" t="s">
+        <v>184</v>
       </c>
       <c r="G13" t="s">
-        <v>185</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>182</v>
-      </c>
+        <v>186</v>
+      </c>
+      <c r="H13" s="3"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>97</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>171</v>
+        <v>96</v>
+      </c>
+      <c r="E14" t="s">
+        <v>170</v>
+      </c>
+      <c r="F14" t="s">
+        <v>184</v>
       </c>
       <c r="G14" t="s">
-        <v>185</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>182</v>
-      </c>
+        <v>186</v>
+      </c>
+      <c r="H14" s="3"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C15" t="s">
         <v>97</v>
@@ -3279,7 +3521,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C16" t="s">
         <v>97</v>
@@ -3299,7 +3541,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C17" t="s">
         <v>97</v>
@@ -3319,7 +3561,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C18" t="s">
         <v>97</v>
@@ -3339,7 +3581,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C19" t="s">
         <v>97</v>
@@ -3359,46 +3601,50 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C20" t="s">
-        <v>98</v>
-      </c>
-      <c r="E20" t="s">
-        <v>169</v>
+        <v>97</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>171</v>
       </c>
       <c r="G20" t="s">
-        <v>186</v>
-      </c>
-      <c r="H20" s="3"/>
+        <v>185</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C21" t="s">
-        <v>99</v>
-      </c>
-      <c r="E21" t="s">
-        <v>169</v>
+        <v>97</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>171</v>
       </c>
       <c r="G21" t="s">
-        <v>186</v>
-      </c>
-      <c r="H21" s="3"/>
+        <v>185</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C22" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E22" t="s">
         <v>169</v>
@@ -3413,62 +3659,52 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C23" t="s">
-        <v>101</v>
-      </c>
-      <c r="D23" t="s">
-        <v>93</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>170</v>
+        <v>99</v>
+      </c>
+      <c r="E23" t="s">
+        <v>169</v>
       </c>
       <c r="G23" t="s">
-        <v>185</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>182</v>
-      </c>
+        <v>186</v>
+      </c>
+      <c r="H23" s="3"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C24" t="s">
-        <v>102</v>
-      </c>
-      <c r="D24" t="s">
-        <v>93</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>172</v>
+        <v>100</v>
+      </c>
+      <c r="E24" t="s">
+        <v>169</v>
       </c>
       <c r="G24" t="s">
-        <v>185</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>182</v>
-      </c>
+        <v>186</v>
+      </c>
+      <c r="H24" s="3"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C25" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D25" t="s">
         <v>93</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G25" t="s">
         <v>185</v>
@@ -3482,101 +3718,107 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C26" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D26" t="s">
         <v>93</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="F26" t="s">
-        <v>209</v>
+      <c r="E26" s="4" t="s">
+        <v>172</v>
       </c>
       <c r="G26" t="s">
         <v>185</v>
       </c>
-      <c r="H26" s="3"/>
+      <c r="H26" s="3" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C27" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D27" t="s">
         <v>93</v>
       </c>
-      <c r="E27" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="F27" t="s">
-        <v>209</v>
+      <c r="E27" s="4" t="s">
+        <v>172</v>
       </c>
       <c r="G27" t="s">
         <v>185</v>
       </c>
-      <c r="H27" s="3"/>
+      <c r="H27" s="3" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C28" t="s">
-        <v>106</v>
-      </c>
-      <c r="E28" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D28" t="s">
+        <v>93</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>170</v>
+      </c>
+      <c r="F28" t="s">
+        <v>209</v>
       </c>
       <c r="G28" t="s">
         <v>185</v>
       </c>
-      <c r="H28" s="3" t="s">
-        <v>182</v>
-      </c>
+      <c r="H28" s="3"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C29" t="s">
-        <v>107</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>172</v>
+        <v>105</v>
+      </c>
+      <c r="D29" t="s">
+        <v>93</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F29" t="s">
+        <v>209</v>
       </c>
       <c r="G29" t="s">
         <v>185</v>
       </c>
-      <c r="H29" s="3" t="s">
-        <v>182</v>
-      </c>
+      <c r="H29" s="3"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C30" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G30" t="s">
         <v>185</v>
@@ -3590,16 +3832,13 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C31" t="s">
-        <v>109</v>
-      </c>
-      <c r="D31" t="s">
-        <v>110</v>
-      </c>
-      <c r="E31" t="s">
-        <v>167</v>
+        <v>107</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>172</v>
       </c>
       <c r="G31" t="s">
         <v>185</v>
@@ -3613,16 +3852,13 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C32" t="s">
-        <v>111</v>
-      </c>
-      <c r="D32" t="s">
-        <v>110</v>
-      </c>
-      <c r="E32" t="s">
-        <v>167</v>
+        <v>108</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>172</v>
       </c>
       <c r="G32" t="s">
         <v>185</v>
@@ -3636,22 +3872,22 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C33" t="s">
-        <v>112</v>
+        <v>109</v>
+      </c>
+      <c r="D33" t="s">
+        <v>110</v>
       </c>
       <c r="E33" t="s">
-        <v>173</v>
-      </c>
-      <c r="F33" t="s">
-        <v>113</v>
+        <v>167</v>
       </c>
       <c r="G33" t="s">
         <v>185</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -3659,137 +3895,98 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C34" t="s">
-        <v>114</v>
+        <v>111</v>
+      </c>
+      <c r="D34" t="s">
+        <v>110</v>
       </c>
       <c r="E34" t="s">
-        <v>173</v>
-      </c>
-      <c r="F34" t="s">
-        <v>113</v>
+        <v>167</v>
       </c>
       <c r="G34" t="s">
         <v>185</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35" t="s">
-        <v>33</v>
-      </c>
-      <c r="C35" t="s">
-        <v>115</v>
-      </c>
-      <c r="E35" t="s">
-        <v>174</v>
-      </c>
-      <c r="F35" t="s">
-        <v>116</v>
-      </c>
-      <c r="G35" t="s">
-        <v>185</v>
-      </c>
-      <c r="H35" s="3" t="s">
-        <v>189</v>
-      </c>
+      <c r="B35" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="3"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36" t="s">
-        <v>34</v>
-      </c>
-      <c r="C36" t="s">
-        <v>117</v>
-      </c>
-      <c r="E36" t="s">
-        <v>174</v>
-      </c>
-      <c r="F36" t="s">
-        <v>116</v>
-      </c>
-      <c r="G36" t="s">
-        <v>185</v>
-      </c>
-      <c r="H36" s="3" t="s">
-        <v>190</v>
-      </c>
+      <c r="B36" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="3"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37" t="s">
-        <v>35</v>
-      </c>
-      <c r="C37" t="s">
-        <v>118</v>
-      </c>
-      <c r="E37" t="s">
-        <v>174</v>
-      </c>
-      <c r="F37" t="s">
-        <v>116</v>
-      </c>
-      <c r="G37" t="s">
-        <v>185</v>
-      </c>
-      <c r="H37" s="3" t="s">
-        <v>191</v>
-      </c>
+      <c r="B37" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="3"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
-      <c r="B38" t="s">
-        <v>36</v>
-      </c>
-      <c r="C38" t="s">
-        <v>119</v>
-      </c>
-      <c r="E38" t="s">
-        <v>174</v>
-      </c>
-      <c r="F38" t="s">
-        <v>116</v>
-      </c>
-      <c r="G38" t="s">
-        <v>185</v>
-      </c>
-      <c r="H38" s="3" t="s">
-        <v>192</v>
-      </c>
+      <c r="B38" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="3"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C39" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="E39" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F39" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="G39" t="s">
         <v>185</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -3797,103 +3994,114 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C40" t="s">
-        <v>122</v>
-      </c>
-      <c r="D40" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="E40" t="s">
-        <v>169</v>
+        <v>173</v>
+      </c>
+      <c r="F40" t="s">
+        <v>113</v>
       </c>
       <c r="G40" t="s">
-        <v>186</v>
-      </c>
-      <c r="H40" s="3"/>
+        <v>185</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C41" t="s">
-        <v>124</v>
-      </c>
-      <c r="D41" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="E41" t="s">
-        <v>169</v>
+        <v>174</v>
+      </c>
+      <c r="F41" t="s">
+        <v>116</v>
       </c>
       <c r="G41" t="s">
-        <v>186</v>
-      </c>
-      <c r="H41" s="3"/>
+        <v>185</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C42" t="s">
-        <v>126</v>
-      </c>
-      <c r="D42" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="E42" t="s">
-        <v>169</v>
+        <v>174</v>
+      </c>
+      <c r="F42" t="s">
+        <v>116</v>
       </c>
       <c r="G42" t="s">
-        <v>186</v>
-      </c>
-      <c r="H42" s="3"/>
+        <v>185</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C43" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="E43" t="s">
-        <v>169</v>
+        <v>174</v>
+      </c>
+      <c r="F43" t="s">
+        <v>116</v>
       </c>
       <c r="G43" t="s">
-        <v>186</v>
-      </c>
-      <c r="H43" s="3"/>
+        <v>185</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C44" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="E44" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F44" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="G44" t="s">
         <v>185</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -3901,22 +4109,22 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C45" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="E45" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F45" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="G45" t="s">
         <v>185</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -3924,114 +4132,103 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C46" t="s">
-        <v>132</v>
+        <v>122</v>
+      </c>
+      <c r="D46" t="s">
+        <v>123</v>
       </c>
       <c r="E46" t="s">
-        <v>178</v>
-      </c>
-      <c r="F46" t="s">
-        <v>133</v>
+        <v>169</v>
       </c>
       <c r="G46" t="s">
-        <v>185</v>
-      </c>
-      <c r="H46" s="3" t="s">
-        <v>195</v>
-      </c>
+        <v>186</v>
+      </c>
+      <c r="H46" s="3"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C47" t="s">
-        <v>134</v>
+        <v>124</v>
+      </c>
+      <c r="D47" t="s">
+        <v>125</v>
       </c>
       <c r="E47" t="s">
-        <v>178</v>
-      </c>
-      <c r="F47" t="s">
-        <v>133</v>
+        <v>169</v>
       </c>
       <c r="G47" t="s">
-        <v>185</v>
-      </c>
-      <c r="H47" s="3" t="s">
-        <v>195</v>
-      </c>
+        <v>186</v>
+      </c>
+      <c r="H47" s="3"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C48" t="s">
-        <v>135</v>
+        <v>126</v>
+      </c>
+      <c r="D48" t="s">
+        <v>125</v>
       </c>
       <c r="E48" t="s">
-        <v>179</v>
-      </c>
-      <c r="F48" t="s">
-        <v>136</v>
+        <v>169</v>
       </c>
       <c r="G48" t="s">
-        <v>185</v>
-      </c>
-      <c r="H48" s="3" t="s">
-        <v>196</v>
-      </c>
+        <v>186</v>
+      </c>
+      <c r="H48" s="3"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C49" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="E49" t="s">
-        <v>178</v>
-      </c>
-      <c r="F49" t="s">
-        <v>133</v>
+        <v>169</v>
       </c>
       <c r="G49" t="s">
-        <v>185</v>
-      </c>
-      <c r="H49" s="3" t="s">
-        <v>197</v>
-      </c>
+        <v>186</v>
+      </c>
+      <c r="H49" s="3"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C50" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="E50" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F50" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G50" t="s">
         <v>185</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -4039,19 +4236,22 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C51" t="s">
-        <v>139</v>
+        <v>130</v>
+      </c>
+      <c r="E51" t="s">
+        <v>177</v>
       </c>
       <c r="F51" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="G51" t="s">
         <v>185</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -4059,10 +4259,10 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C52" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="E52" t="s">
         <v>178</v>
@@ -4074,7 +4274,7 @@
         <v>185</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -4082,10 +4282,10 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C53" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="E53" t="s">
         <v>178</v>
@@ -4097,7 +4297,7 @@
         <v>185</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -4105,22 +4305,22 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C54" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="E54" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F54" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="G54" t="s">
         <v>185</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -4128,22 +4328,19 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C55" t="s">
-        <v>144</v>
-      </c>
-      <c r="E55" t="s">
-        <v>178</v>
+        <v>139</v>
       </c>
       <c r="F55" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="G55" t="s">
         <v>185</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -4151,94 +4348,111 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C56" t="s">
-        <v>145</v>
-      </c>
-      <c r="D56" t="s">
-        <v>123</v>
+        <v>141</v>
       </c>
       <c r="E56" t="s">
-        <v>169</v>
+        <v>178</v>
+      </c>
+      <c r="F56" t="s">
+        <v>133</v>
       </c>
       <c r="G56" t="s">
-        <v>186</v>
-      </c>
-      <c r="H56" s="3"/>
+        <v>185</v>
+      </c>
+      <c r="H56" s="3" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C57" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E57" t="s">
-        <v>169</v>
+        <v>178</v>
+      </c>
+      <c r="F57" t="s">
+        <v>133</v>
       </c>
       <c r="G57" t="s">
-        <v>186</v>
-      </c>
-      <c r="H57" s="3"/>
+        <v>185</v>
+      </c>
+      <c r="H57" s="3" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C58" t="s">
-        <v>147</v>
-      </c>
-      <c r="D58" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
       <c r="E58" t="s">
-        <v>169</v>
+        <v>178</v>
+      </c>
+      <c r="F58" t="s">
+        <v>133</v>
       </c>
       <c r="G58" t="s">
-        <v>186</v>
-      </c>
-      <c r="H58" s="3"/>
+        <v>185</v>
+      </c>
+      <c r="H58" s="3" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C59" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E59" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F59" t="s">
-        <v>149</v>
-      </c>
-      <c r="H59" s="3"/>
+        <v>133</v>
+      </c>
+      <c r="G59" t="s">
+        <v>185</v>
+      </c>
+      <c r="H59" s="3" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C60" t="s">
-        <v>150</v>
+        <v>145</v>
+      </c>
+      <c r="D60" t="s">
+        <v>123</v>
       </c>
       <c r="E60" t="s">
-        <v>180</v>
-      </c>
-      <c r="F60" t="s">
-        <v>149</v>
+        <v>169</v>
+      </c>
+      <c r="G60" t="s">
+        <v>186</v>
       </c>
       <c r="H60" s="3"/>
     </row>
@@ -4247,16 +4461,16 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C61" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E61" t="s">
-        <v>180</v>
-      </c>
-      <c r="F61" t="s">
-        <v>149</v>
+        <v>169</v>
+      </c>
+      <c r="G61" t="s">
+        <v>186</v>
       </c>
       <c r="H61" s="3"/>
     </row>
@@ -4265,16 +4479,19 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C62" t="s">
-        <v>151</v>
+        <v>147</v>
+      </c>
+      <c r="D62" t="s">
+        <v>125</v>
       </c>
       <c r="E62" t="s">
-        <v>180</v>
-      </c>
-      <c r="F62" t="s">
-        <v>149</v>
+        <v>169</v>
+      </c>
+      <c r="G62" t="s">
+        <v>186</v>
       </c>
       <c r="H62" s="3"/>
     </row>
@@ -4283,7 +4500,7 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C63" t="s">
         <v>148</v>
@@ -4301,10 +4518,10 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C64" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E64" t="s">
         <v>180</v>
@@ -4319,7 +4536,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C65" t="s">
         <v>148</v>
@@ -4337,10 +4554,10 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C66" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E66" t="s">
         <v>180</v>
@@ -4355,7 +4572,7 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C67" t="s">
         <v>148</v>
@@ -4373,10 +4590,10 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C68" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E68" t="s">
         <v>180</v>
@@ -4391,7 +4608,7 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C69" t="s">
         <v>148</v>
@@ -4409,10 +4626,10 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C70" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E70" t="s">
         <v>180</v>
@@ -4427,7 +4644,7 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C71" t="s">
         <v>148</v>
@@ -4445,10 +4662,10 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C72" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E72" t="s">
         <v>180</v>
@@ -4463,7 +4680,7 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C73" t="s">
         <v>148</v>
@@ -4481,10 +4698,10 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C74" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E74" t="s">
         <v>180</v>
@@ -4499,90 +4716,82 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C75" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="E75" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="F75" t="s">
-        <v>159</v>
-      </c>
-      <c r="H75" s="3" t="s">
-        <v>187</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="H75" s="3"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C76" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E76" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="F76" t="s">
-        <v>159</v>
-      </c>
-      <c r="H76" s="3" t="s">
-        <v>188</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="H76" s="3"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C77" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="E77" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="F77" t="s">
-        <v>159</v>
-      </c>
-      <c r="H77" s="3" t="s">
-        <v>189</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="H77" s="3"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C78" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="E78" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="F78" t="s">
-        <v>159</v>
-      </c>
-      <c r="H78" s="3" t="s">
-        <v>190</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="H78" s="3"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C79" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="E79" t="s">
         <v>169</v>
@@ -4591,7 +4800,7 @@
         <v>159</v>
       </c>
       <c r="H79" s="3" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -4599,10 +4808,10 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>164</v>
+        <v>74</v>
       </c>
       <c r="C80" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="E80" t="s">
         <v>169</v>
@@ -4611,7 +4820,7 @@
         <v>159</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -4619,10 +4828,10 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C81" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="E81" t="s">
         <v>169</v>
@@ -4631,14 +4840,298 @@
         <v>159</v>
       </c>
       <c r="H81" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" s="2">
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
+        <v>76</v>
+      </c>
+      <c r="C82" t="s">
+        <v>162</v>
+      </c>
+      <c r="E82" t="s">
+        <v>169</v>
+      </c>
+      <c r="F82" t="s">
+        <v>159</v>
+      </c>
+      <c r="H82" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" s="2">
+        <v>82</v>
+      </c>
+      <c r="B83" t="s">
+        <v>77</v>
+      </c>
+      <c r="C83" t="s">
+        <v>163</v>
+      </c>
+      <c r="E83" t="s">
+        <v>169</v>
+      </c>
+      <c r="F83" t="s">
+        <v>159</v>
+      </c>
+      <c r="H83" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" s="2">
+        <v>83</v>
+      </c>
+      <c r="B84" t="s">
+        <v>164</v>
+      </c>
+      <c r="C84" t="s">
+        <v>165</v>
+      </c>
+      <c r="E84" t="s">
+        <v>169</v>
+      </c>
+      <c r="F84" t="s">
+        <v>159</v>
+      </c>
+      <c r="H84" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" s="2">
+        <v>84</v>
+      </c>
+      <c r="B85" t="s">
+        <v>79</v>
+      </c>
+      <c r="C85" t="s">
+        <v>166</v>
+      </c>
+      <c r="E85" t="s">
+        <v>169</v>
+      </c>
+      <c r="F85" t="s">
+        <v>159</v>
+      </c>
+      <c r="H85" s="3" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A82" s="2"/>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="2">
+        <v>85</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" s="2">
+        <v>86</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" s="2">
+        <v>87</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" s="2">
+        <v>88</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C89" s="5"/>
+      <c r="E89" s="5"/>
+      <c r="F89" s="5"/>
+      <c r="G89" s="5"/>
+      <c r="H89" s="5"/>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" s="2">
+        <v>89</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C90" s="5"/>
+      <c r="E90" s="5"/>
+      <c r="F90" s="5"/>
+      <c r="G90" s="5"/>
+      <c r="H90" s="5"/>
+    </row>
+    <row r="91" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="2">
+        <v>90</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="2">
+        <v>91</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="2">
+        <v>92</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="2">
+        <v>93</v>
+      </c>
+      <c r="B94" s="5" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="2">
+        <v>94</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="2">
+        <v>95</v>
+      </c>
+      <c r="B96" s="5" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="2">
+        <v>96</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="2">
+        <v>97</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="2">
+        <v>98</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="2">
+        <v>99</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="2">
+        <v>100</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="C101"/>
+      <c r="E101"/>
+      <c r="F101"/>
+      <c r="G101"/>
+      <c r="H101"/>
+    </row>
+    <row r="102" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="2">
+        <v>101</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="C102"/>
+      <c r="E102"/>
+      <c r="F102"/>
+      <c r="G102"/>
+      <c r="H102"/>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>54</v>
+      </c>
+      <c r="B105" t="s">
+        <v>47</v>
+      </c>
+      <c r="C105" t="s">
+        <v>137</v>
+      </c>
+      <c r="E105" t="s">
+        <v>178</v>
+      </c>
+      <c r="F105" t="s">
+        <v>133</v>
+      </c>
+      <c r="G105" t="s">
+        <v>185</v>
+      </c>
+      <c r="H105" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>55</v>
+      </c>
+      <c r="B106" t="s">
+        <v>48</v>
+      </c>
+      <c r="C106" t="s">
+        <v>138</v>
+      </c>
+      <c r="E106" t="s">
+        <v>178</v>
+      </c>
+      <c r="F106" t="s">
+        <v>133</v>
+      </c>
+      <c r="G106" t="s">
+        <v>185</v>
+      </c>
+      <c r="H106" t="s">
+        <v>197</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="H1:H81"/>
+  <autoFilter ref="H1:H85"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update of SUEWSPrepare (v2019a) and SUEWSConverter
</commit_message>
<xml_diff>
--- a/SUEWSPrepare/Input/SUEWS_SiteSelect.xlsx
+++ b/SUEWSPrepare/Input/SUEWS_SiteSelect.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xlinfr\Documents\PythonScripts\UMEP\SUEWSPrepare\Input\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="345" windowWidth="18690" windowHeight="8835"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16005" windowHeight="6690"/>
   </bookViews>
   <sheets>
     <sheet name="SUEWS_SiteSelect" sheetId="1" r:id="rId1"/>
@@ -13,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Metadata!$H$1:$H$85</definedName>
   </definedNames>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -746,8 +751,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -882,6 +887,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="35">
@@ -1237,13 +1247,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1295,6 +1306,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1342,7 +1356,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1377,7 +1391,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1589,7 +1603,7 @@
   <dimension ref="A1:CZ67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2394,13 +2408,13 @@
         <v>14.2</v>
       </c>
       <c r="AC3" s="5">
-        <v>-999</v>
+        <v>0.3</v>
       </c>
       <c r="AD3" s="5">
-        <v>-999</v>
+        <v>0.3</v>
       </c>
       <c r="AE3" s="5">
-        <v>-999</v>
+        <v>0.3</v>
       </c>
       <c r="AF3" s="5">
         <v>-999</v>
@@ -2843,10 +2857,14 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:104" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>80</v>
-      </c>
+    <row r="7" spans="1:104" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="G7" s="6"/>
     </row>
     <row r="8" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A8" t="s">

</xml_diff>

<commit_message>
3.11.1: Response to issues #96, #125, #129 and #130. Configuring for gdal3. New plugin DownloadData (ERA5).
</commit_message>
<xml_diff>
--- a/SUEWSPrepare/Input/SUEWS_SiteSelect.xlsx
+++ b/SUEWSPrepare/Input/SUEWS_SiteSelect.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="243">
   <si>
     <t>Grid</t>
   </si>
@@ -746,6 +746,12 @@
   </si>
   <si>
     <t>old</t>
+  </si>
+  <si>
+    <t>TrafficRate_WD</t>
+  </si>
+  <si>
+    <t>TrafficRate_WE</t>
   </si>
 </sst>
 </file>
@@ -1602,8 +1608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CZ67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AI2" sqref="AI2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2109,10 +2115,10 @@
         <v>30</v>
       </c>
       <c r="AH2" s="5" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
       <c r="AI2" s="5" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="AJ2" s="5" t="s">
         <v>238</v>

</xml_diff>

<commit_message>
3.14  : LONG TERM RELEASE
Updated with SUEWS v2020a. Response to issues #158, #160 and #162.
</commit_message>
<xml_diff>
--- a/SUEWSPrepare/Input/SUEWS_SiteSelect.xlsx
+++ b/SUEWSPrepare/Input/SUEWS_SiteSelect.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16005" windowHeight="6690"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9336"/>
   </bookViews>
   <sheets>
     <sheet name="SUEWS_SiteSelect" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="247">
   <si>
     <t>Grid</t>
   </si>
@@ -752,6 +752,18 @@
   </si>
   <si>
     <t>TrafficRate_WE</t>
+  </si>
+  <si>
+    <t>IrrFr_Paved</t>
+  </si>
+  <si>
+    <t>IrrFr_Bldgs</t>
+  </si>
+  <si>
+    <t>IrrFr_BSoil</t>
+  </si>
+  <si>
+    <t>IrrFr_Water</t>
   </si>
 </sst>
 </file>
@@ -1606,117 +1618,121 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CZ67"/>
+  <dimension ref="A1:DD61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="AI2" sqref="AI2"/>
+    <sheetView tabSelected="1" topLeftCell="CM1" workbookViewId="0">
+      <selection activeCell="CQ7" sqref="CQ7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="13.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="5" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="5" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="15" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="12" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="12" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="15" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="20" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="19" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="22" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="19" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="12" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="19" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="12" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="19" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="12" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="19" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="12" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="19" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="12" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="19" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="12" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="19" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="12" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="19" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="12" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="21" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="21" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="86" max="88" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="89" max="91" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="92" max="96" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="97" max="101" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="102" max="102" width="1.7109375" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="8" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="4" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="14" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="11" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="11" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="19.77734375" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="19" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="90" max="92" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="93" max="95" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="96" max="100" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="101" max="105" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="1.6640625" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="38.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:104" x14ac:dyDescent="0.25">
-      <c r="A1" s="5">
+    <row r="1" spans="1:108" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6">
         <v>1</v>
       </c>
-      <c r="B1" s="5">
+      <c r="B1" s="6">
         <v>2</v>
       </c>
-      <c r="C1" s="5">
+      <c r="C1" s="6">
         <v>3</v>
       </c>
-      <c r="D1" s="5">
+      <c r="D1" s="6">
         <v>4</v>
       </c>
       <c r="E1" s="5">
@@ -1725,7 +1741,7 @@
       <c r="F1" s="5">
         <v>6</v>
       </c>
-      <c r="G1" s="5">
+      <c r="G1" s="6">
         <v>7</v>
       </c>
       <c r="H1" s="5">
@@ -2010,1165 +2026,958 @@
       <c r="CW1" s="5">
         <v>101</v>
       </c>
-      <c r="CX1" s="5"/>
-      <c r="CY1" s="5"/>
-      <c r="CZ1" s="5"/>
-    </row>
-    <row r="2" spans="1:104" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="CX1" s="5">
+        <v>102</v>
+      </c>
+      <c r="CY1" s="5">
+        <v>103</v>
+      </c>
+      <c r="CZ1" s="5">
+        <v>104</v>
+      </c>
+      <c r="DA1" s="5">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:108" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" t="s">
         <v>235</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" t="s">
         <v>236</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="O2" t="s">
         <v>12</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="P2" t="s">
         <v>13</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="Q2" t="s">
         <v>14</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="R2" t="s">
         <v>15</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="S2" t="s">
         <v>16</v>
       </c>
-      <c r="T2" s="5" t="s">
+      <c r="T2" t="s">
         <v>17</v>
       </c>
-      <c r="U2" s="5" t="s">
+      <c r="U2" t="s">
+        <v>243</v>
+      </c>
+      <c r="V2" t="s">
+        <v>244</v>
+      </c>
+      <c r="W2" t="s">
         <v>18</v>
       </c>
-      <c r="V2" s="5" t="s">
+      <c r="X2" t="s">
         <v>19</v>
       </c>
-      <c r="W2" s="5" t="s">
+      <c r="Y2" t="s">
         <v>20</v>
       </c>
-      <c r="X2" s="5" t="s">
+      <c r="Z2" t="s">
+        <v>245</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>246</v>
+      </c>
+      <c r="AB2" t="s">
         <v>21</v>
       </c>
-      <c r="Y2" s="5" t="s">
+      <c r="AC2" t="s">
         <v>22</v>
       </c>
-      <c r="Z2" s="5" t="s">
+      <c r="AD2" t="s">
         <v>23</v>
       </c>
-      <c r="AA2" s="5" t="s">
+      <c r="AE2" t="s">
         <v>24</v>
       </c>
-      <c r="AB2" s="5" t="s">
+      <c r="AF2" t="s">
         <v>25</v>
       </c>
-      <c r="AC2" s="5" t="s">
+      <c r="AG2" t="s">
         <v>26</v>
       </c>
-      <c r="AD2" s="5" t="s">
+      <c r="AH2" t="s">
         <v>27</v>
       </c>
-      <c r="AE2" s="5" t="s">
+      <c r="AI2" t="s">
         <v>28</v>
       </c>
-      <c r="AF2" s="5" t="s">
+      <c r="AJ2" t="s">
         <v>29</v>
       </c>
-      <c r="AG2" s="5" t="s">
+      <c r="AK2" t="s">
         <v>30</v>
       </c>
-      <c r="AH2" s="5" t="s">
+      <c r="AL2" t="s">
         <v>241</v>
       </c>
-      <c r="AI2" s="5" t="s">
+      <c r="AM2" t="s">
         <v>242</v>
       </c>
-      <c r="AJ2" s="5" t="s">
+      <c r="AN2" t="s">
         <v>238</v>
       </c>
-      <c r="AK2" s="5" t="s">
+      <c r="AO2" t="s">
         <v>239</v>
       </c>
-      <c r="AL2" s="5" t="s">
+      <c r="AP2" t="s">
         <v>31</v>
       </c>
-      <c r="AM2" s="5" t="s">
+      <c r="AQ2" t="s">
         <v>32</v>
       </c>
-      <c r="AN2" s="5" t="s">
+      <c r="AR2" t="s">
         <v>33</v>
       </c>
-      <c r="AO2" s="5" t="s">
+      <c r="AS2" t="s">
         <v>34</v>
       </c>
-      <c r="AP2" s="5" t="s">
+      <c r="AT2" t="s">
         <v>35</v>
       </c>
-      <c r="AQ2" s="5" t="s">
+      <c r="AU2" t="s">
         <v>36</v>
       </c>
-      <c r="AR2" s="5" t="s">
+      <c r="AV2" t="s">
         <v>37</v>
       </c>
-      <c r="AS2" s="5" t="s">
+      <c r="AW2" t="s">
         <v>38</v>
       </c>
-      <c r="AT2" s="5" t="s">
+      <c r="AX2" t="s">
         <v>39</v>
       </c>
-      <c r="AU2" s="5" t="s">
+      <c r="AY2" t="s">
         <v>40</v>
       </c>
-      <c r="AV2" s="5" t="s">
+      <c r="AZ2" t="s">
         <v>41</v>
       </c>
-      <c r="AW2" s="5" t="s">
+      <c r="BA2" t="s">
         <v>42</v>
       </c>
-      <c r="AX2" s="5" t="s">
+      <c r="BB2" t="s">
         <v>43</v>
       </c>
-      <c r="AY2" s="5" t="s">
+      <c r="BC2" t="s">
         <v>44</v>
       </c>
-      <c r="AZ2" s="5" t="s">
+      <c r="BD2" t="s">
         <v>45</v>
       </c>
-      <c r="BA2" s="5" t="s">
+      <c r="BE2" t="s">
         <v>46</v>
       </c>
-      <c r="BB2" s="5" t="s">
+      <c r="BF2" t="s">
         <v>49</v>
       </c>
-      <c r="BC2" s="5" t="s">
+      <c r="BG2" t="s">
         <v>50</v>
       </c>
-      <c r="BD2" s="5" t="s">
+      <c r="BH2" t="s">
         <v>51</v>
       </c>
-      <c r="BE2" s="5" t="s">
+      <c r="BI2" t="s">
         <v>52</v>
       </c>
-      <c r="BF2" s="5" t="s">
+      <c r="BJ2" t="s">
         <v>53</v>
       </c>
-      <c r="BG2" s="5" t="s">
+      <c r="BK2" t="s">
         <v>54</v>
       </c>
-      <c r="BH2" s="5" t="s">
+      <c r="BL2" t="s">
         <v>55</v>
       </c>
-      <c r="BI2" s="5" t="s">
+      <c r="BM2" t="s">
         <v>56</v>
       </c>
-      <c r="BJ2" s="5" t="s">
+      <c r="BN2" t="s">
         <v>57</v>
       </c>
-      <c r="BK2" s="5" t="s">
+      <c r="BO2" t="s">
         <v>58</v>
       </c>
-      <c r="BL2" s="5" t="s">
+      <c r="BP2" t="s">
         <v>59</v>
       </c>
-      <c r="BM2" s="5" t="s">
+      <c r="BQ2" t="s">
         <v>60</v>
       </c>
-      <c r="BN2" s="5" t="s">
+      <c r="BR2" t="s">
         <v>61</v>
       </c>
-      <c r="BO2" s="5" t="s">
+      <c r="BS2" t="s">
         <v>62</v>
       </c>
-      <c r="BP2" s="5" t="s">
+      <c r="BT2" t="s">
         <v>63</v>
       </c>
-      <c r="BQ2" s="5" t="s">
+      <c r="BU2" t="s">
         <v>64</v>
       </c>
-      <c r="BR2" s="5" t="s">
+      <c r="BV2" t="s">
         <v>65</v>
       </c>
-      <c r="BS2" s="5" t="s">
+      <c r="BW2" t="s">
         <v>66</v>
       </c>
-      <c r="BT2" s="5" t="s">
+      <c r="BX2" t="s">
         <v>67</v>
       </c>
-      <c r="BU2" s="5" t="s">
+      <c r="BY2" t="s">
         <v>68</v>
       </c>
-      <c r="BV2" s="5" t="s">
+      <c r="BZ2" t="s">
         <v>69</v>
       </c>
-      <c r="BW2" s="5" t="s">
+      <c r="CA2" t="s">
         <v>70</v>
       </c>
-      <c r="BX2" s="5" t="s">
+      <c r="CB2" t="s">
         <v>71</v>
       </c>
-      <c r="BY2" s="5" t="s">
+      <c r="CC2" t="s">
         <v>72</v>
       </c>
-      <c r="BZ2" s="5" t="s">
+      <c r="CD2" t="s">
         <v>73</v>
       </c>
-      <c r="CA2" s="5" t="s">
+      <c r="CE2" t="s">
         <v>74</v>
       </c>
-      <c r="CB2" s="5" t="s">
+      <c r="CF2" t="s">
         <v>75</v>
       </c>
-      <c r="CC2" s="5" t="s">
+      <c r="CG2" t="s">
         <v>76</v>
       </c>
-      <c r="CD2" s="5" t="s">
+      <c r="CH2" t="s">
         <v>77</v>
       </c>
-      <c r="CE2" s="5" t="s">
+      <c r="CI2" t="s">
         <v>78</v>
       </c>
-      <c r="CF2" s="5" t="s">
+      <c r="CJ2" t="s">
         <v>79</v>
       </c>
-      <c r="CG2" s="5" t="s">
+      <c r="CK2" t="s">
         <v>214</v>
       </c>
-      <c r="CH2" s="5" t="s">
+      <c r="CL2" t="s">
         <v>215</v>
       </c>
-      <c r="CI2" s="5" t="s">
+      <c r="CM2" t="s">
         <v>216</v>
       </c>
-      <c r="CJ2" s="5" t="s">
+      <c r="CN2" t="s">
         <v>217</v>
       </c>
-      <c r="CK2" s="5" t="s">
+      <c r="CO2" t="s">
         <v>218</v>
       </c>
-      <c r="CL2" s="5" t="s">
+      <c r="CP2" t="s">
         <v>219</v>
       </c>
-      <c r="CM2" s="5" t="s">
+      <c r="CQ2" t="s">
         <v>220</v>
       </c>
-      <c r="CN2" s="5" t="s">
+      <c r="CR2" t="s">
         <v>221</v>
       </c>
-      <c r="CO2" s="5" t="s">
+      <c r="CS2" t="s">
         <v>222</v>
       </c>
-      <c r="CP2" s="5" t="s">
+      <c r="CT2" t="s">
         <v>223</v>
       </c>
-      <c r="CQ2" s="5" t="s">
+      <c r="CU2" t="s">
         <v>224</v>
       </c>
-      <c r="CR2" s="5" t="s">
+      <c r="CV2" t="s">
         <v>225</v>
       </c>
-      <c r="CS2" s="5" t="s">
+      <c r="CW2" t="s">
         <v>226</v>
       </c>
-      <c r="CT2" s="5" t="s">
+      <c r="CX2" t="s">
         <v>227</v>
       </c>
-      <c r="CU2" s="5" t="s">
+      <c r="CY2" t="s">
         <v>228</v>
       </c>
-      <c r="CV2" s="5" t="s">
+      <c r="CZ2" t="s">
         <v>229</v>
       </c>
-      <c r="CW2" s="5" t="s">
+      <c r="DA2" t="s">
         <v>230</v>
       </c>
-      <c r="CX2" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="CY2" s="5" t="s">
+      <c r="DB2" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="DC2" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="CZ2" s="5" t="s">
+      <c r="DD2" s="5" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="3" spans="1:104" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>98</v>
-      </c>
-      <c r="B3" s="5">
-        <v>2012</v>
-      </c>
-      <c r="C3" s="5">
-        <v>85</v>
-      </c>
-      <c r="D3" s="5">
-        <v>302</v>
-      </c>
-      <c r="E3" s="5">
+    <row r="3" spans="1:108" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2011</v>
+      </c>
+      <c r="C3">
+        <v>86</v>
+      </c>
+      <c r="D3">
+        <v>303</v>
+      </c>
+      <c r="E3">
         <v>51.51</v>
       </c>
-      <c r="F3" s="5">
-        <v>0.12</v>
-      </c>
-      <c r="G3" s="5">
+      <c r="F3">
+        <v>-0.12</v>
+      </c>
+      <c r="G3">
         <v>0</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3">
         <v>2221.56</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3">
         <v>10.7</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3">
         <v>49.6</v>
       </c>
-      <c r="K3" s="5">
+      <c r="K3">
         <v>1</v>
       </c>
-      <c r="L3" s="5">
+      <c r="L3">
         <v>0</v>
       </c>
-      <c r="M3" s="5">
+      <c r="M3">
         <v>0</v>
       </c>
-      <c r="N3" s="5">
+      <c r="N3">
         <v>0.43</v>
       </c>
-      <c r="O3" s="5">
+      <c r="O3">
         <v>0.38</v>
       </c>
-      <c r="P3" s="5">
+      <c r="P3">
         <v>0</v>
       </c>
-      <c r="Q3" s="5">
+      <c r="Q3">
         <v>0.02</v>
       </c>
-      <c r="R3" s="5">
+      <c r="R3">
         <v>0.03</v>
       </c>
-      <c r="S3" s="5">
+      <c r="S3">
         <v>0</v>
       </c>
-      <c r="T3" s="5">
+      <c r="T3">
         <v>0.14000000000000001</v>
       </c>
-      <c r="U3" s="5">
+      <c r="U3">
         <v>0</v>
       </c>
-      <c r="V3" s="5">
+      <c r="V3">
         <v>0</v>
       </c>
-      <c r="W3" s="5">
+      <c r="W3">
         <v>0</v>
       </c>
-      <c r="X3" s="5">
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3">
         <v>22</v>
       </c>
-      <c r="Y3" s="5">
+      <c r="AC3">
         <v>13.1</v>
       </c>
-      <c r="Z3" s="5">
+      <c r="AD3">
         <v>13.1</v>
       </c>
-      <c r="AA3" s="5">
+      <c r="AE3">
         <v>1.9</v>
       </c>
-      <c r="AB3" s="5">
+      <c r="AF3">
         <v>14.2</v>
       </c>
-      <c r="AC3" s="5">
+      <c r="AG3">
         <v>0.3</v>
       </c>
-      <c r="AD3" s="5">
+      <c r="AH3">
         <v>0.3</v>
       </c>
-      <c r="AE3" s="5">
+      <c r="AI3">
         <v>0.3</v>
       </c>
-      <c r="AF3" s="5">
-        <v>-999</v>
-      </c>
-      <c r="AG3" s="5">
+      <c r="AJ3">
         <v>204.58</v>
       </c>
-      <c r="AH3" s="5">
-        <v>-999</v>
-      </c>
-      <c r="AI3" s="5">
-        <v>-999</v>
-      </c>
-      <c r="AJ3" s="5">
+      <c r="AK3">
+        <v>204.58</v>
+      </c>
+      <c r="AL3">
+        <v>0.01</v>
+      </c>
+      <c r="AM3">
+        <v>0.01</v>
+      </c>
+      <c r="AN3">
         <v>0.88</v>
       </c>
-      <c r="AK3" s="5">
+      <c r="AO3">
         <v>0.88</v>
       </c>
-      <c r="AL3" s="5">
+      <c r="AP3">
         <v>661</v>
       </c>
-      <c r="AM3" s="5">
+      <c r="AQ3">
         <v>662</v>
       </c>
-      <c r="AN3" s="5">
+      <c r="AR3">
         <v>661</v>
       </c>
-      <c r="AO3" s="5">
+      <c r="AS3">
         <v>662</v>
       </c>
-      <c r="AP3" s="5">
+      <c r="AT3">
         <v>663</v>
       </c>
-      <c r="AQ3" s="5">
+      <c r="AU3">
         <v>663</v>
       </c>
-      <c r="AR3" s="5">
+      <c r="AV3">
         <v>661</v>
       </c>
-      <c r="AS3" s="5">
+      <c r="AW3">
         <v>0.25</v>
       </c>
-      <c r="AT3" s="5">
+      <c r="AX3">
         <v>1</v>
       </c>
-      <c r="AU3" s="5">
+      <c r="AY3">
         <v>10</v>
       </c>
-      <c r="AV3" s="5">
+      <c r="AZ3">
         <v>1</v>
       </c>
-      <c r="AW3" s="5">
+      <c r="BA3">
         <v>200</v>
       </c>
-      <c r="AX3" s="5">
-        <v>99999</v>
-      </c>
-      <c r="AY3" s="5">
-        <v>99999</v>
-      </c>
-      <c r="AZ3" s="5">
-        <v>99999</v>
-      </c>
-      <c r="BA3" s="5">
+      <c r="BB3">
+        <v>999</v>
+      </c>
+      <c r="BC3">
+        <v>999</v>
+      </c>
+      <c r="BD3">
+        <v>999</v>
+      </c>
+      <c r="BE3">
         <v>661</v>
       </c>
-      <c r="BB3" s="5">
-        <v>99999</v>
-      </c>
-      <c r="BC3" s="5">
-        <v>99999</v>
-      </c>
-      <c r="BD3" s="5">
-        <v>99999</v>
-      </c>
-      <c r="BE3" s="5">
-        <v>99999</v>
-      </c>
-      <c r="BF3" s="5">
-        <v>99999</v>
-      </c>
-      <c r="BG3" s="5">
+      <c r="BF3">
+        <v>999</v>
+      </c>
+      <c r="BG3">
+        <v>999</v>
+      </c>
+      <c r="BH3">
+        <v>999</v>
+      </c>
+      <c r="BI3">
+        <v>999</v>
+      </c>
+      <c r="BJ3">
+        <v>999</v>
+      </c>
+      <c r="BK3">
         <v>0</v>
       </c>
-      <c r="BH3" s="5">
+      <c r="BL3">
         <v>0</v>
       </c>
-      <c r="BI3" s="5">
+      <c r="BM3">
         <v>100</v>
       </c>
-      <c r="BJ3" s="5">
+      <c r="BN3">
         <v>0</v>
       </c>
-      <c r="BK3" s="5">
+      <c r="BO3">
         <v>0</v>
       </c>
-      <c r="BL3" s="5">
+      <c r="BP3">
         <v>0</v>
       </c>
-      <c r="BM3" s="5">
+      <c r="BQ3">
         <v>0</v>
       </c>
-      <c r="BN3" s="5">
+      <c r="BR3">
         <v>0</v>
       </c>
-      <c r="BO3" s="5">
+      <c r="BS3">
         <v>0</v>
       </c>
-      <c r="BP3" s="5">
+      <c r="BT3">
         <v>0</v>
       </c>
-      <c r="BQ3" s="5">
+      <c r="BU3">
         <v>0</v>
       </c>
-      <c r="BR3" s="5">
+      <c r="BV3">
         <v>0</v>
       </c>
-      <c r="BS3" s="5">
+      <c r="BW3">
         <v>0</v>
       </c>
-      <c r="BT3" s="5">
+      <c r="BX3">
         <v>0</v>
       </c>
-      <c r="BU3" s="5">
+      <c r="BY3">
         <v>0</v>
       </c>
-      <c r="BV3" s="5">
+      <c r="BZ3">
         <v>0</v>
       </c>
-      <c r="BW3" s="5">
+      <c r="CA3">
         <v>0</v>
       </c>
-      <c r="BX3" s="5">
+      <c r="CB3">
         <v>0</v>
       </c>
-      <c r="BY3" s="5">
+      <c r="CC3">
         <v>0</v>
       </c>
-      <c r="BZ3" s="5">
+      <c r="CD3">
         <v>661</v>
       </c>
-      <c r="CA3" s="5">
+      <c r="CE3">
         <v>662</v>
       </c>
-      <c r="CB3" s="5">
+      <c r="CF3">
         <v>663</v>
       </c>
-      <c r="CC3" s="5">
+      <c r="CG3">
         <v>664</v>
       </c>
-      <c r="CD3" s="5">
+      <c r="CH3">
         <v>665</v>
       </c>
-      <c r="CE3" s="5">
+      <c r="CI3">
         <v>666</v>
       </c>
-      <c r="CF3" s="5">
+      <c r="CJ3">
         <v>667</v>
       </c>
-      <c r="CG3" s="5">
-        <v>1.08</v>
-      </c>
-      <c r="CH3" s="5">
-        <v>0.15</v>
-      </c>
-      <c r="CI3" s="5">
-        <v>0.05</v>
-      </c>
-      <c r="CJ3" s="5">
-        <v>0.8</v>
-      </c>
-      <c r="CK3" s="5">
+      <c r="CK3">
+        <v>7000</v>
+      </c>
+      <c r="CL3">
+        <v>0</v>
+      </c>
+      <c r="CM3">
+        <v>1</v>
+      </c>
+      <c r="CN3">
+        <v>0</v>
+      </c>
+      <c r="CO3">
         <v>806</v>
       </c>
-      <c r="CL3" s="5">
+      <c r="CP3">
         <v>807</v>
       </c>
-      <c r="CM3" s="5">
+      <c r="CQ3">
         <v>808</v>
       </c>
-      <c r="CN3" s="5">
-        <v>0.15</v>
-      </c>
-      <c r="CO3" s="5">
-        <v>0.45</v>
-      </c>
-      <c r="CP3" s="5">
-        <v>0.05</v>
-      </c>
-      <c r="CQ3" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="CR3" s="5">
-        <v>0.25</v>
-      </c>
-      <c r="CS3" s="5">
+      <c r="CR3">
+        <v>1</v>
+      </c>
+      <c r="CS3">
+        <v>0</v>
+      </c>
+      <c r="CT3">
+        <v>0</v>
+      </c>
+      <c r="CU3">
+        <v>0</v>
+      </c>
+      <c r="CV3">
+        <v>0</v>
+      </c>
+      <c r="CW3">
         <v>801</v>
       </c>
-      <c r="CT3" s="5">
-        <v>8021</v>
-      </c>
-      <c r="CU3" s="5">
-        <v>8022</v>
-      </c>
-      <c r="CV3" s="5">
+      <c r="CX3">
+        <v>802</v>
+      </c>
+      <c r="CY3">
         <v>803</v>
       </c>
-      <c r="CW3" s="5">
-        <v>8041</v>
-      </c>
-      <c r="CX3" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="CY3" s="5" t="s">
+      <c r="CZ3">
+        <v>804</v>
+      </c>
+      <c r="DA3">
+        <v>805</v>
+      </c>
+      <c r="DB3" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="DC3" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="CZ3" s="5" t="s">
+      <c r="DD3" s="5" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="4" spans="1:104" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+    <row r="4" spans="1:108" x14ac:dyDescent="0.3">
+      <c r="A4">
         <v>-9</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
-      <c r="T4" s="5"/>
-      <c r="U4" s="5"/>
-      <c r="V4" s="5"/>
-      <c r="W4" s="5"/>
-      <c r="X4" s="5"/>
-      <c r="Y4" s="5"/>
-      <c r="Z4" s="5"/>
-      <c r="AA4" s="5"/>
-      <c r="AB4" s="5"/>
-      <c r="AC4" s="5"/>
-      <c r="AD4" s="5"/>
-      <c r="AE4" s="5"/>
-      <c r="AF4" s="5"/>
-      <c r="AG4" s="5"/>
-      <c r="AH4" s="5"/>
-      <c r="AI4" s="5"/>
-      <c r="AJ4" s="5"/>
-      <c r="AK4" s="5"/>
-      <c r="AL4" s="5"/>
-      <c r="AM4" s="5"/>
-      <c r="AN4" s="5"/>
-      <c r="AO4" s="5"/>
-      <c r="AP4" s="5"/>
-      <c r="AQ4" s="5"/>
-      <c r="AR4" s="5"/>
-      <c r="AS4" s="5"/>
-      <c r="AT4" s="5"/>
-      <c r="AU4" s="5"/>
-      <c r="AV4" s="5"/>
-      <c r="AW4" s="5"/>
-      <c r="AX4" s="5"/>
-      <c r="AY4" s="5"/>
-      <c r="AZ4" s="5"/>
-      <c r="BA4" s="5"/>
-      <c r="BB4" s="5"/>
-      <c r="BC4" s="5"/>
-      <c r="BD4" s="5"/>
-      <c r="BE4" s="5"/>
-      <c r="BF4" s="5"/>
-      <c r="BG4" s="5"/>
-      <c r="BH4" s="5"/>
-      <c r="BI4" s="5"/>
-      <c r="BJ4" s="5"/>
-      <c r="BK4" s="5"/>
-      <c r="BL4" s="5"/>
-      <c r="BM4" s="5"/>
-      <c r="BN4" s="5"/>
-      <c r="BO4" s="5"/>
-      <c r="BP4" s="5"/>
-      <c r="BQ4" s="5"/>
-      <c r="BR4" s="5"/>
-      <c r="BS4" s="5"/>
-      <c r="BT4" s="5"/>
-      <c r="BU4" s="5"/>
-      <c r="BV4" s="5"/>
-      <c r="BW4" s="5"/>
-      <c r="BX4" s="5"/>
-      <c r="BY4" s="5"/>
-      <c r="BZ4" s="5"/>
-      <c r="CA4" s="5"/>
-      <c r="CB4" s="5"/>
-      <c r="CC4" s="5"/>
-      <c r="CD4" s="5"/>
-      <c r="CE4" s="5"/>
-      <c r="CF4" s="5"/>
-      <c r="CG4" s="5"/>
-      <c r="CH4" s="5"/>
-      <c r="CI4" s="5"/>
-      <c r="CJ4" s="5"/>
-      <c r="CK4" s="5"/>
-      <c r="CL4" s="5"/>
-      <c r="CM4" s="5"/>
-      <c r="CN4" s="5"/>
-      <c r="CO4" s="5"/>
-      <c r="CP4" s="5"/>
-      <c r="CQ4" s="5"/>
-      <c r="CR4" s="5"/>
-      <c r="CS4" s="5"/>
-      <c r="CT4" s="5"/>
-      <c r="CU4" s="5"/>
-      <c r="CV4" s="5"/>
-      <c r="CW4" s="5"/>
-      <c r="CX4" s="5"/>
-      <c r="CY4" s="5"/>
-      <c r="CZ4" s="5"/>
-    </row>
-    <row r="5" spans="1:104" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+    </row>
+    <row r="5" spans="1:108" x14ac:dyDescent="0.3">
+      <c r="A5">
         <v>-9</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="5"/>
-      <c r="T5" s="5"/>
-      <c r="U5" s="5"/>
-      <c r="V5" s="5"/>
-      <c r="W5" s="5"/>
-      <c r="X5" s="5"/>
-      <c r="Y5" s="5"/>
-      <c r="Z5" s="5"/>
-      <c r="AA5" s="5"/>
-      <c r="AB5" s="5"/>
-      <c r="AC5" s="5"/>
-      <c r="AD5" s="5"/>
-      <c r="AE5" s="5"/>
-      <c r="AF5" s="5"/>
-      <c r="AG5" s="5"/>
-      <c r="AH5" s="5"/>
-      <c r="AI5" s="5"/>
-      <c r="AJ5" s="5"/>
-      <c r="AK5" s="5"/>
-      <c r="AL5" s="5"/>
-      <c r="AM5" s="5"/>
-      <c r="AN5" s="5"/>
-      <c r="AO5" s="5"/>
-      <c r="AP5" s="5"/>
-      <c r="AQ5" s="5"/>
-      <c r="AR5" s="5"/>
-      <c r="AS5" s="5"/>
-      <c r="AT5" s="5"/>
-      <c r="AU5" s="5"/>
-      <c r="AV5" s="5"/>
-      <c r="AW5" s="5"/>
-      <c r="AX5" s="5"/>
-      <c r="AY5" s="5"/>
-      <c r="AZ5" s="5"/>
-      <c r="BA5" s="5"/>
-      <c r="BB5" s="5"/>
-      <c r="BC5" s="5"/>
-      <c r="BD5" s="5"/>
-      <c r="BE5" s="5"/>
-      <c r="BF5" s="5"/>
-      <c r="BG5" s="5"/>
-      <c r="BH5" s="5"/>
-      <c r="BI5" s="5"/>
-      <c r="BJ5" s="5"/>
-      <c r="BK5" s="5"/>
-      <c r="BL5" s="5"/>
-      <c r="BM5" s="5"/>
-      <c r="BN5" s="5"/>
-      <c r="BO5" s="5"/>
-      <c r="BP5" s="5"/>
-      <c r="BQ5" s="5"/>
-      <c r="BR5" s="5"/>
-      <c r="BS5" s="5"/>
-      <c r="BT5" s="5"/>
-      <c r="BU5" s="5"/>
-      <c r="BV5" s="5"/>
-      <c r="BW5" s="5"/>
-      <c r="BX5" s="5"/>
-      <c r="BY5" s="5"/>
-      <c r="BZ5" s="5"/>
-      <c r="CA5" s="5"/>
-      <c r="CB5" s="5"/>
-      <c r="CC5" s="5"/>
-      <c r="CD5" s="5"/>
-      <c r="CE5" s="5"/>
-      <c r="CF5" s="5"/>
-      <c r="CG5" s="5"/>
-      <c r="CH5" s="5"/>
-      <c r="CI5" s="5"/>
-      <c r="CJ5" s="5"/>
-      <c r="CK5" s="5"/>
-      <c r="CL5" s="5"/>
-      <c r="CM5" s="5"/>
-      <c r="CN5" s="5"/>
-      <c r="CO5" s="5"/>
-      <c r="CP5" s="5"/>
-      <c r="CQ5" s="5"/>
-      <c r="CR5" s="5"/>
-      <c r="CS5" s="5"/>
-      <c r="CT5" s="5"/>
-      <c r="CU5" s="5"/>
-      <c r="CV5" s="5"/>
-      <c r="CW5" s="5"/>
-      <c r="CX5" s="5"/>
-      <c r="CY5" s="5"/>
-      <c r="CZ5" s="5"/>
-    </row>
-    <row r="6" spans="1:104" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:108" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:104" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="G7" s="6"/>
-    </row>
-    <row r="8" spans="1:104" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:108" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:108" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:104" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:108" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:104" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:108" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:104" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:108" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:104" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:108" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:104" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:108" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:104" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:108" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:104" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:108" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:104" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:108" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
         <v>80</v>
       </c>
     </row>
@@ -3186,20 +2995,20 @@
       <selection activeCell="F91" sqref="F91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="54" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="54" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" customWidth="1"/>
-    <col min="6" max="6" width="33.85546875" customWidth="1"/>
-    <col min="7" max="7" width="20.85546875" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" customWidth="1"/>
-    <col min="9" max="9" width="21.28515625" customWidth="1"/>
-    <col min="10" max="40" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" customWidth="1"/>
+    <col min="4" max="4" width="19.88671875" customWidth="1"/>
+    <col min="5" max="5" width="26.109375" customWidth="1"/>
+    <col min="6" max="6" width="33.88671875" customWidth="1"/>
+    <col min="7" max="7" width="20.88671875" customWidth="1"/>
+    <col min="8" max="8" width="15.88671875" customWidth="1"/>
+    <col min="9" max="9" width="21.33203125" customWidth="1"/>
+    <col min="10" max="40" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>200</v>
       </c>
@@ -3225,7 +3034,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3251,7 +3060,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3274,7 +3083,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -3297,7 +3106,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -3320,7 +3129,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3346,7 +3155,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3372,7 +3181,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3387,7 +3196,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="5"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3413,7 +3222,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3439,7 +3248,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3454,7 +3263,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="5"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3478,7 +3287,7 @@
       </c>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3499,7 +3308,7 @@
       </c>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3520,7 +3329,7 @@
       </c>
       <c r="H14" s="3"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3540,7 +3349,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3560,7 +3369,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3580,7 +3389,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3600,7 +3409,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3620,7 +3429,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -3640,7 +3449,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -3660,7 +3469,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -3678,7 +3487,7 @@
       </c>
       <c r="H22" s="3"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3696,7 +3505,7 @@
       </c>
       <c r="H23" s="3"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3714,7 +3523,7 @@
       </c>
       <c r="H24" s="3"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3737,7 +3546,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3760,7 +3569,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3783,7 +3592,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3807,7 +3616,7 @@
       </c>
       <c r="H28" s="3"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3831,7 +3640,7 @@
       </c>
       <c r="H29" s="3"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3851,7 +3660,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3871,7 +3680,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3891,7 +3700,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3914,7 +3723,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3937,7 +3746,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3948,7 +3757,7 @@
       <c r="G35" s="5"/>
       <c r="H35" s="3"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3962,7 +3771,7 @@
       <c r="G36" s="5"/>
       <c r="H36" s="3"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3976,7 +3785,7 @@
       <c r="G37" s="5"/>
       <c r="H37" s="3"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3990,7 +3799,7 @@
       <c r="G38" s="5"/>
       <c r="H38" s="3"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -4013,7 +3822,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -4036,7 +3845,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -4059,7 +3868,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -4082,7 +3891,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -4105,7 +3914,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -4128,7 +3937,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -4151,7 +3960,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -4172,7 +3981,7 @@
       </c>
       <c r="H46" s="3"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -4193,7 +4002,7 @@
       </c>
       <c r="H47" s="3"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -4214,7 +4023,7 @@
       </c>
       <c r="H48" s="3"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -4232,7 +4041,7 @@
       </c>
       <c r="H49" s="3"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -4255,7 +4064,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -4278,7 +4087,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -4301,7 +4110,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -4324,7 +4133,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -4347,7 +4156,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -4367,7 +4176,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -4390,7 +4199,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -4413,7 +4222,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -4436,7 +4245,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
@@ -4459,7 +4268,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -4480,7 +4289,7 @@
       </c>
       <c r="H60" s="3"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
@@ -4498,7 +4307,7 @@
       </c>
       <c r="H61" s="3"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
@@ -4519,7 +4328,7 @@
       </c>
       <c r="H62" s="3"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
@@ -4537,7 +4346,7 @@
       </c>
       <c r="H63" s="3"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
@@ -4555,7 +4364,7 @@
       </c>
       <c r="H64" s="3"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>64</v>
       </c>
@@ -4573,7 +4382,7 @@
       </c>
       <c r="H65" s="3"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>65</v>
       </c>
@@ -4591,7 +4400,7 @@
       </c>
       <c r="H66" s="3"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>66</v>
       </c>
@@ -4609,7 +4418,7 @@
       </c>
       <c r="H67" s="3"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>67</v>
       </c>
@@ -4627,7 +4436,7 @@
       </c>
       <c r="H68" s="3"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>68</v>
       </c>
@@ -4645,7 +4454,7 @@
       </c>
       <c r="H69" s="3"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>69</v>
       </c>
@@ -4663,7 +4472,7 @@
       </c>
       <c r="H70" s="3"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>70</v>
       </c>
@@ -4681,7 +4490,7 @@
       </c>
       <c r="H71" s="3"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>71</v>
       </c>
@@ -4699,7 +4508,7 @@
       </c>
       <c r="H72" s="3"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>72</v>
       </c>
@@ -4717,7 +4526,7 @@
       </c>
       <c r="H73" s="3"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>73</v>
       </c>
@@ -4735,7 +4544,7 @@
       </c>
       <c r="H74" s="3"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" s="2">
         <v>74</v>
       </c>
@@ -4753,7 +4562,7 @@
       </c>
       <c r="H75" s="3"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" s="2">
         <v>75</v>
       </c>
@@ -4771,7 +4580,7 @@
       </c>
       <c r="H76" s="3"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" s="2">
         <v>76</v>
       </c>
@@ -4789,7 +4598,7 @@
       </c>
       <c r="H77" s="3"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" s="2">
         <v>77</v>
       </c>
@@ -4807,7 +4616,7 @@
       </c>
       <c r="H78" s="3"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" s="2">
         <v>78</v>
       </c>
@@ -4827,7 +4636,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="2">
         <v>79</v>
       </c>
@@ -4847,7 +4656,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" s="2">
         <v>80</v>
       </c>
@@ -4867,7 +4676,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" s="2">
         <v>81</v>
       </c>
@@ -4887,7 +4696,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" s="2">
         <v>82</v>
       </c>
@@ -4907,7 +4716,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" s="2">
         <v>83</v>
       </c>
@@ -4927,7 +4736,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" s="2">
         <v>84</v>
       </c>
@@ -4947,7 +4756,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" s="2">
         <v>85</v>
       </c>
@@ -4955,7 +4764,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" s="2">
         <v>86</v>
       </c>
@@ -4963,7 +4772,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" s="2">
         <v>87</v>
       </c>
@@ -4971,7 +4780,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" s="2">
         <v>88</v>
       </c>
@@ -4984,7 +4793,7 @@
       <c r="G89" s="5"/>
       <c r="H89" s="5"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" s="2">
         <v>89</v>
       </c>
@@ -4997,7 +4806,7 @@
       <c r="G90" s="5"/>
       <c r="H90" s="5"/>
     </row>
-    <row r="91" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A91" s="2">
         <v>90</v>
       </c>
@@ -5005,7 +4814,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="92" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A92" s="2">
         <v>91</v>
       </c>
@@ -5013,7 +4822,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="93" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A93" s="2">
         <v>92</v>
       </c>
@@ -5021,7 +4830,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="94" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A94" s="2">
         <v>93</v>
       </c>
@@ -5029,7 +4838,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="95" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A95" s="2">
         <v>94</v>
       </c>
@@ -5037,7 +4846,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="96" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A96" s="2">
         <v>95</v>
       </c>
@@ -5045,7 +4854,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="97" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A97" s="2">
         <v>96</v>
       </c>
@@ -5053,7 +4862,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="98" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A98" s="2">
         <v>97</v>
       </c>
@@ -5061,7 +4870,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="99" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A99" s="2">
         <v>98</v>
       </c>
@@ -5069,7 +4878,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="100" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A100" s="2">
         <v>99</v>
       </c>
@@ -5077,7 +4886,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="101" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A101" s="2">
         <v>100</v>
       </c>
@@ -5090,7 +4899,7 @@
       <c r="G101"/>
       <c r="H101"/>
     </row>
-    <row r="102" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A102" s="2">
         <v>101</v>
       </c>
@@ -5103,12 +4912,12 @@
       <c r="G102"/>
       <c r="H102"/>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>54</v>
       </c>
@@ -5131,7 +4940,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>55</v>
       </c>

</xml_diff>